<commit_message>
add two core paper and revise original main file
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="363">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="364">
   <si>
     <t>Period</t>
   </si>
@@ -1105,6 +1105,9 @@
   </si>
   <si>
     <t>HFRI EH</t>
+  </si>
+  <si>
+    <t>HFRI_Fixed_Income</t>
   </si>
 </sst>
 </file>
@@ -1161,7 +1164,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
@@ -1169,6 +1172,9 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="10" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -1504,11 +1510,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M350"/>
+  <dimension ref="A1:N350"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M27" sqref="M27:M350"/>
+      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="N1" sqref="N1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1522,7 +1528,7 @@
     <col min="7" max="7" width="6.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1562,8 +1568,11 @@
       <c r="M1" t="s">
         <v>362</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N1" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -1574,7 +1583,7 @@
         <v>7.3700000000000002E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -1588,7 +1597,7 @@
         <v>4.4699999999999997E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -1602,7 +1611,7 @@
         <v>5.2299999999999999E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -1616,7 +1625,7 @@
         <v>-2.0400000000000001E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -1630,7 +1639,7 @@
         <v>9.4000000000000004E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
@@ -1644,7 +1653,7 @@
         <v>3.3E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
@@ -1658,7 +1667,7 @@
         <v>5.28E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
@@ -1672,7 +1681,7 @@
         <v>-8.0000000000000002E-3</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
@@ -1686,7 +1695,7 @@
         <v>-2.7699999999999999E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
@@ -1700,7 +1709,7 @@
         <v>4.02E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
@@ -1714,7 +1723,7 @@
         <v>1.84E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>12</v>
       </c>
@@ -1728,7 +1737,7 @@
         <v>-1.6799999999999999E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>13</v>
       </c>
@@ -1742,7 +1751,7 @@
         <v>2.1399999999999999E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>14</v>
       </c>
@@ -1756,7 +1765,7 @@
         <v>6.7299999999999999E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>15</v>
       </c>
@@ -1770,7 +1779,7 @@
         <v>-1.7600000000000001E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>16</v>
       </c>
@@ -1784,7 +1793,7 @@
         <v>2.2700000000000001E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>17</v>
       </c>
@@ -1798,7 +1807,7 @@
         <v>5.0099999999999999E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>18</v>
       </c>
@@ -1812,7 +1821,7 @@
         <v>4.2700000000000002E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>19</v>
       </c>
@@ -1826,7 +1835,7 @@
         <v>-6.4999999999999997E-3</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>20</v>
       </c>
@@ -1840,7 +1849,7 @@
         <v>8.0399999999999999E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>21</v>
       </c>
@@ -1854,7 +1863,7 @@
         <v>2.0899999999999998E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>22</v>
       </c>
@@ -1868,7 +1877,7 @@
         <v>-2.0999999999999999E-3</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>23</v>
       </c>
@@ -1882,7 +1891,7 @@
         <v>-2.9100000000000001E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>24</v>
       </c>
@@ -1896,7 +1905,7 @@
         <v>1.7999999999999999E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>25</v>
       </c>
@@ -1910,7 +1919,7 @@
         <v>1.9E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>26</v>
       </c>
@@ -1938,8 +1947,11 @@
       <c r="M27" s="15">
         <v>1.23E-2</v>
       </c>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N27" s="16">
+        <v>-1.47E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>27</v>
       </c>
@@ -1967,8 +1979,11 @@
       <c r="M28" s="15">
         <v>1.23E-2</v>
       </c>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N28" s="16">
+        <v>-9.1999999999999998E-3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>28</v>
       </c>
@@ -1996,8 +2011,11 @@
       <c r="M29" s="15">
         <v>8.2000000000000007E-3</v>
       </c>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N29" s="16">
+        <v>1.26E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>29</v>
       </c>
@@ -2025,8 +2043,11 @@
       <c r="M30" s="15">
         <v>7.3000000000000001E-3</v>
       </c>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N30" s="16">
+        <v>1.4800000000000001E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>30</v>
       </c>
@@ -2054,8 +2075,11 @@
       <c r="M31" s="15">
         <v>5.0000000000000001E-3</v>
       </c>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N31" s="16">
+        <v>1.7500000000000002E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>31</v>
       </c>
@@ -2083,8 +2107,11 @@
       <c r="M32" s="15">
         <v>1.37E-2</v>
       </c>
-    </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N32" s="16">
+        <v>1.72E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>32</v>
       </c>
@@ -2112,8 +2139,11 @@
       <c r="M33" s="15">
         <v>7.7000000000000002E-3</v>
       </c>
-    </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N33" s="16">
+        <v>1.15E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>33</v>
       </c>
@@ -2141,8 +2171,11 @@
       <c r="M34" s="15">
         <v>1.7999999999999999E-2</v>
       </c>
-    </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N34" s="16">
+        <v>-1.8E-3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>34</v>
       </c>
@@ -2170,8 +2203,11 @@
       <c r="M35" s="15">
         <v>1.8100000000000002E-2</v>
       </c>
-    </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N35" s="16">
+        <v>-4.7000000000000002E-3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>35</v>
       </c>
@@ -2199,8 +2235,11 @@
       <c r="M36" s="15">
         <v>1.37E-2</v>
       </c>
-    </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N36" s="16">
+        <v>-1.5599999999999999E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>36</v>
       </c>
@@ -2228,8 +2267,11 @@
       <c r="M37" s="15">
         <v>8.3000000000000001E-3</v>
       </c>
-    </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N37" s="16">
+        <v>-5.0000000000000001E-4</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>37</v>
       </c>
@@ -2257,8 +2299,11 @@
       <c r="M38" s="15">
         <v>2.01E-2</v>
       </c>
-    </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N38" s="16">
+        <v>-4.8999999999999998E-3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>38</v>
       </c>
@@ -2286,8 +2331,11 @@
       <c r="M39" s="15">
         <v>2.5100000000000001E-2</v>
       </c>
-    </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N39" s="16">
+        <v>4.4000000000000003E-3</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>39</v>
       </c>
@@ -2315,8 +2363,11 @@
       <c r="M40" s="15">
         <v>4.0000000000000002E-4</v>
       </c>
-    </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N40" s="16">
+        <v>1.61E-2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>40</v>
       </c>
@@ -2344,8 +2395,11 @@
       <c r="M41" s="15">
         <v>2.7E-2</v>
       </c>
-    </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N41" s="16">
+        <v>1.3899999999999999E-2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>41</v>
       </c>
@@ -2373,8 +2427,11 @@
       <c r="M42" s="15">
         <v>-1E-4</v>
       </c>
-    </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N42" s="16">
+        <v>1.49E-2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>42</v>
       </c>
@@ -2402,8 +2459,11 @@
       <c r="M43" s="15">
         <v>-2.0000000000000001E-4</v>
       </c>
-    </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N43" s="16">
+        <v>9.4000000000000004E-3</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>43</v>
       </c>
@@ -2431,8 +2491,11 @@
       <c r="M44" s="15">
         <v>5.5999999999999999E-3</v>
       </c>
-    </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N44" s="16">
+        <v>9.7999999999999997E-3</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>44</v>
       </c>
@@ -2460,8 +2523,11 @@
       <c r="M45" s="15">
         <v>2.5000000000000001E-2</v>
       </c>
-    </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N45" s="16">
+        <v>1.5699999999999999E-2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>45</v>
       </c>
@@ -2489,8 +2555,11 @@
       <c r="M46" s="15">
         <v>2.8E-3</v>
       </c>
-    </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N46" s="16">
+        <v>2.0899999999999998E-2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>46</v>
       </c>
@@ -2518,8 +2587,11 @@
       <c r="M47" s="15">
         <v>1.9199999999999998E-2</v>
       </c>
-    </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N47" s="16">
+        <v>1.3100000000000001E-2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>47</v>
       </c>
@@ -2547,8 +2619,11 @@
       <c r="M48" s="15">
         <v>9.7000000000000003E-3</v>
       </c>
-    </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N48" s="16">
+        <v>1.2200000000000001E-2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>48</v>
       </c>
@@ -2576,8 +2651,11 @@
       <c r="M49" s="15">
         <v>1.17E-2</v>
       </c>
-    </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N49" s="16">
+        <v>1.66E-2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>49</v>
       </c>
@@ -2605,8 +2683,11 @@
       <c r="M50" s="15">
         <v>2.07E-2</v>
       </c>
-    </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N50" s="16">
+        <v>1.6299999999999999E-2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>50</v>
       </c>
@@ -2634,8 +2715,11 @@
       <c r="M51" s="15">
         <v>3.5999999999999999E-3</v>
       </c>
-    </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N51" s="16">
+        <v>2.12E-2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>51</v>
       </c>
@@ -2663,8 +2747,11 @@
       <c r="M52" s="15">
         <v>9.5999999999999992E-3</v>
       </c>
-    </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N52" s="16">
+        <v>9.4000000000000004E-3</v>
+      </c>
+    </row>
+    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>52</v>
       </c>
@@ -2692,8 +2779,11 @@
       <c r="M53" s="15">
         <v>5.7999999999999996E-3</v>
       </c>
-    </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N53" s="16">
+        <v>9.9000000000000008E-3</v>
+      </c>
+    </row>
+    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>53</v>
       </c>
@@ -2721,8 +2811,11 @@
       <c r="M54" s="15">
         <v>-2.9999999999999997E-4</v>
       </c>
-    </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N54" s="16">
+        <v>8.0000000000000002E-3</v>
+      </c>
+    </row>
+    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>54</v>
       </c>
@@ -2750,8 +2843,11 @@
       <c r="M55" s="15">
         <v>1.1000000000000001E-3</v>
       </c>
-    </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N55" s="16">
+        <v>1.7000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>55</v>
       </c>
@@ -2779,8 +2875,11 @@
       <c r="M56" s="15">
         <v>6.1999999999999998E-3</v>
       </c>
-    </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N56" s="16">
+        <v>7.1000000000000004E-3</v>
+      </c>
+    </row>
+    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>56</v>
       </c>
@@ -2808,8 +2907,11 @@
       <c r="M57" s="15">
         <v>1.24E-2</v>
       </c>
-    </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N57" s="16">
+        <v>1.8499999999999999E-2</v>
+      </c>
+    </row>
+    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>57</v>
       </c>
@@ -2837,8 +2939,11 @@
       <c r="M58" s="15">
         <v>-3.5000000000000001E-3</v>
       </c>
-    </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N58" s="16">
+        <v>1.6500000000000001E-2</v>
+      </c>
+    </row>
+    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>58</v>
       </c>
@@ -2866,8 +2971,11 @@
       <c r="M59" s="15">
         <v>1.17E-2</v>
       </c>
-    </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N59" s="16">
+        <v>1.46E-2</v>
+      </c>
+    </row>
+    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>59</v>
       </c>
@@ -2895,8 +3003,11 @@
       <c r="M60" s="15">
         <v>1.04E-2</v>
       </c>
-    </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N60" s="16">
+        <v>1.24E-2</v>
+      </c>
+    </row>
+    <row r="61" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>60</v>
       </c>
@@ -2924,8 +3035,11 @@
       <c r="M61" s="15">
         <v>1.18E-2</v>
       </c>
-    </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N61" s="16">
+        <v>7.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="62" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>61</v>
       </c>
@@ -2953,8 +3067,11 @@
       <c r="M62" s="15">
         <v>1.54E-2</v>
       </c>
-    </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N62" s="16">
+        <v>1.09E-2</v>
+      </c>
+    </row>
+    <row r="63" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>62</v>
       </c>
@@ -2982,8 +3099,11 @@
       <c r="M63" s="15">
         <v>1.9099999999999999E-2</v>
       </c>
-    </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N63" s="16">
+        <v>9.2999999999999992E-3</v>
+      </c>
+    </row>
+    <row r="64" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>63</v>
       </c>
@@ -3011,8 +3131,11 @@
       <c r="M64" s="15">
         <v>1.06E-2</v>
       </c>
-    </row>
-    <row r="65" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N64" s="16">
+        <v>8.6E-3</v>
+      </c>
+    </row>
+    <row r="65" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>64</v>
       </c>
@@ -3040,8 +3163,11 @@
       <c r="M65" s="15">
         <v>1.67E-2</v>
       </c>
-    </row>
-    <row r="66" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N65" s="16">
+        <v>2.1899999999999999E-2</v>
+      </c>
+    </row>
+    <row r="66" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>65</v>
       </c>
@@ -3069,8 +3195,11 @@
       <c r="M66" s="15">
         <v>-1.4E-3</v>
       </c>
-    </row>
-    <row r="67" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N66" s="16">
+        <v>1.4999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="67" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>66</v>
       </c>
@@ -3098,8 +3227,11 @@
       <c r="M67" s="15">
         <v>5.7999999999999996E-3</v>
       </c>
-    </row>
-    <row r="68" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N67" s="16">
+        <v>1.24E-2</v>
+      </c>
+    </row>
+    <row r="68" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>67</v>
       </c>
@@ -3127,8 +3259,11 @@
       <c r="M68" s="15">
         <v>2.3699999999999999E-2</v>
       </c>
-    </row>
-    <row r="69" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N68" s="16">
+        <v>1.04E-2</v>
+      </c>
+    </row>
+    <row r="69" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
         <v>68</v>
       </c>
@@ -3156,8 +3291,11 @@
       <c r="M69" s="15">
         <v>6.3E-3</v>
       </c>
-    </row>
-    <row r="70" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N69" s="16">
+        <v>1.41E-2</v>
+      </c>
+    </row>
+    <row r="70" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>69</v>
       </c>
@@ -3185,8 +3323,11 @@
       <c r="M70" s="15">
         <v>9.1000000000000004E-3</v>
       </c>
-    </row>
-    <row r="71" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N70" s="16">
+        <v>1.4E-2</v>
+      </c>
+    </row>
+    <row r="71" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
         <v>70</v>
       </c>
@@ -3214,8 +3355,11 @@
       <c r="M71" s="15">
         <v>2.4400000000000002E-2</v>
       </c>
-    </row>
-    <row r="72" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N71" s="16">
+        <v>1.03E-2</v>
+      </c>
+    </row>
+    <row r="72" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
         <v>71</v>
       </c>
@@ -3243,8 +3387,11 @@
       <c r="M72" s="15">
         <v>-1E-3</v>
       </c>
-    </row>
-    <row r="73" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N72" s="16">
+        <v>1.29E-2</v>
+      </c>
+    </row>
+    <row r="73" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
         <v>72</v>
       </c>
@@ -3272,8 +3419,11 @@
       <c r="M73" s="15">
         <v>-1.4500000000000001E-2</v>
       </c>
-    </row>
-    <row r="74" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N73" s="16">
+        <v>6.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="74" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
         <v>73</v>
       </c>
@@ -3301,8 +3451,11 @@
       <c r="M74" s="15">
         <v>7.7000000000000002E-3</v>
       </c>
-    </row>
-    <row r="75" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N74" s="16">
+        <v>7.7000000000000002E-3</v>
+      </c>
+    </row>
+    <row r="75" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
         <v>74</v>
       </c>
@@ -3330,8 +3483,11 @@
       <c r="M75" s="15">
         <v>7.7999999999999996E-3</v>
       </c>
-    </row>
-    <row r="76" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N75" s="16">
+        <v>6.6E-3</v>
+      </c>
+    </row>
+    <row r="76" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
         <v>75</v>
       </c>
@@ -3359,8 +3515,11 @@
       <c r="M76" s="15">
         <v>5.7999999999999996E-3</v>
       </c>
-    </row>
-    <row r="77" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N76" s="16">
+        <v>2.3999999999999998E-3</v>
+      </c>
+    </row>
+    <row r="77" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
         <v>76</v>
       </c>
@@ -3388,8 +3547,11 @@
       <c r="M77" s="15">
         <v>4.4000000000000003E-3</v>
       </c>
-    </row>
-    <row r="78" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N77" s="16">
+        <v>-2.1100000000000001E-2</v>
+      </c>
+    </row>
+    <row r="78" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
         <v>77</v>
       </c>
@@ -3417,8 +3579,11 @@
       <c r="M78" s="15">
         <v>9.1999999999999998E-3</v>
       </c>
-    </row>
-    <row r="79" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N78" s="16">
+        <v>-2.7900000000000001E-2</v>
+      </c>
+    </row>
+    <row r="79" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
         <v>78</v>
       </c>
@@ -3446,8 +3611,11 @@
       <c r="M79" s="15">
         <v>-9.4999999999999998E-3</v>
       </c>
-    </row>
-    <row r="80" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N79" s="16">
+        <v>2.9999999999999997E-4</v>
+      </c>
+    </row>
+    <row r="80" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
         <v>79</v>
       </c>
@@ -3475,8 +3643,11 @@
       <c r="M80" s="15">
         <v>5.7999999999999996E-3</v>
       </c>
-    </row>
-    <row r="81" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N80" s="16">
+        <v>1.5E-3</v>
+      </c>
+    </row>
+    <row r="81" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
         <v>80</v>
       </c>
@@ -3504,8 +3675,11 @@
       <c r="M81" s="15">
         <v>3.7000000000000002E-3</v>
       </c>
-    </row>
-    <row r="82" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N81" s="16">
+        <v>1.55E-2</v>
+      </c>
+    </row>
+    <row r="82" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
         <v>81</v>
       </c>
@@ -3533,8 +3707,11 @@
       <c r="M82" s="15">
         <v>-3.5000000000000001E-3</v>
       </c>
-    </row>
-    <row r="83" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N82" s="16">
+        <v>8.0000000000000002E-3</v>
+      </c>
+    </row>
+    <row r="83" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
         <v>82</v>
       </c>
@@ -3562,8 +3739,11 @@
       <c r="M83" s="15">
         <v>2.0000000000000001E-4</v>
       </c>
-    </row>
-    <row r="84" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N83" s="16">
+        <v>1.1999999999999999E-3</v>
+      </c>
+    </row>
+    <row r="84" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
         <v>83</v>
       </c>
@@ -3591,8 +3771,11 @@
       <c r="M84" s="15">
         <v>-1.1999999999999999E-3</v>
       </c>
-    </row>
-    <row r="85" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N84" s="16">
+        <v>-8.9999999999999998E-4</v>
+      </c>
+    </row>
+    <row r="85" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
         <v>84</v>
       </c>
@@ -3620,8 +3803,11 @@
       <c r="M85" s="15">
         <v>-4.4999999999999997E-3</v>
       </c>
-    </row>
-    <row r="86" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N85" s="16">
+        <v>-7.9000000000000008E-3</v>
+      </c>
+    </row>
+    <row r="86" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
         <v>85</v>
       </c>
@@ -3649,8 +3835,11 @@
       <c r="M86" s="15">
         <v>8.2000000000000007E-3</v>
       </c>
-    </row>
-    <row r="87" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N86" s="16">
+        <v>-1.4800000000000001E-2</v>
+      </c>
+    </row>
+    <row r="87" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
         <v>86</v>
       </c>
@@ -3678,8 +3867,11 @@
       <c r="M87" s="15">
         <v>2.2000000000000001E-3</v>
       </c>
-    </row>
-    <row r="88" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N87" s="16">
+        <v>5.4999999999999997E-3</v>
+      </c>
+    </row>
+    <row r="88" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
         <v>87</v>
       </c>
@@ -3707,8 +3899,11 @@
       <c r="M88" s="15">
         <v>1.4200000000000001E-2</v>
       </c>
-    </row>
-    <row r="89" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N88" s="16">
+        <v>9.7999999999999997E-3</v>
+      </c>
+    </row>
+    <row r="89" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
         <v>88</v>
       </c>
@@ -3736,8 +3931,11 @@
       <c r="M89" s="15">
         <v>1.77E-2</v>
       </c>
-    </row>
-    <row r="90" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N89" s="16">
+        <v>1.83E-2</v>
+      </c>
+    </row>
+    <row r="90" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
         <v>89</v>
       </c>
@@ -3765,8 +3963,11 @@
       <c r="M90" s="15">
         <v>1.8599999999999998E-2</v>
       </c>
-    </row>
-    <row r="91" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N90" s="16">
+        <v>1.9E-2</v>
+      </c>
+    </row>
+    <row r="91" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
         <v>90</v>
       </c>
@@ -3794,8 +3995,11 @@
       <c r="M91" s="15">
         <v>6.0000000000000001E-3</v>
       </c>
-    </row>
-    <row r="92" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N91" s="16">
+        <v>1.8800000000000001E-2</v>
+      </c>
+    </row>
+    <row r="92" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
         <v>91</v>
       </c>
@@ -3823,8 +4027,11 @@
       <c r="M92" s="15">
         <v>9.1999999999999998E-3</v>
       </c>
-    </row>
-    <row r="93" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N92" s="16">
+        <v>2.3199999999999998E-2</v>
+      </c>
+    </row>
+    <row r="93" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
         <v>92</v>
       </c>
@@ -3852,8 +4059,11 @@
       <c r="M93" s="15">
         <v>2.23E-2</v>
       </c>
-    </row>
-    <row r="94" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N93" s="16">
+        <v>2.1299999999999999E-2</v>
+      </c>
+    </row>
+    <row r="94" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
         <v>93</v>
       </c>
@@ -3881,8 +4091,11 @@
       <c r="M94" s="15">
         <v>9.7999999999999997E-3</v>
       </c>
-    </row>
-    <row r="95" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N94" s="16">
+        <v>9.5999999999999992E-3</v>
+      </c>
+    </row>
+    <row r="95" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
         <v>94</v>
       </c>
@@ -3910,8 +4123,11 @@
       <c r="M95" s="15">
         <v>1.8499999999999999E-2</v>
       </c>
-    </row>
-    <row r="96" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N95" s="16">
+        <v>1.55E-2</v>
+      </c>
+    </row>
+    <row r="96" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
         <v>95</v>
       </c>
@@ -3939,8 +4155,11 @@
       <c r="M96" s="15">
         <v>1.5800000000000002E-2</v>
       </c>
-    </row>
-    <row r="97" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N96" s="16">
+        <v>1.2500000000000001E-2</v>
+      </c>
+    </row>
+    <row r="97" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
         <v>96</v>
       </c>
@@ -3968,8 +4187,11 @@
       <c r="M97" s="15">
         <v>7.7999999999999996E-3</v>
       </c>
-    </row>
-    <row r="98" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N97" s="16">
+        <v>1.5800000000000002E-2</v>
+      </c>
+    </row>
+    <row r="98" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
         <v>97</v>
       </c>
@@ -3997,8 +4219,11 @@
       <c r="M98" s="15">
         <v>1.03E-2</v>
       </c>
-    </row>
-    <row r="99" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N98" s="16">
+        <v>1.3299999999999999E-2</v>
+      </c>
+    </row>
+    <row r="99" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
         <v>98</v>
       </c>
@@ -4026,8 +4251,11 @@
       <c r="M99" s="15">
         <v>2.18E-2</v>
       </c>
-    </row>
-    <row r="100" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N99" s="16">
+        <v>1.8200000000000001E-2</v>
+      </c>
+    </row>
+    <row r="100" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
         <v>99</v>
       </c>
@@ -4055,8 +4283,11 @@
       <c r="M100" s="15">
         <v>9.4999999999999998E-3</v>
       </c>
-    </row>
-    <row r="101" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N100" s="16">
+        <v>1.06E-2</v>
+      </c>
+    </row>
+    <row r="101" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
         <v>100</v>
       </c>
@@ -4084,8 +4315,11 @@
       <c r="M101" s="15">
         <v>8.6E-3</v>
       </c>
-    </row>
-    <row r="102" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N101" s="16">
+        <v>1.17E-2</v>
+      </c>
+    </row>
+    <row r="102" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
         <v>101</v>
       </c>
@@ -4113,8 +4347,11 @@
       <c r="M102" s="15">
         <v>3.5000000000000001E-3</v>
       </c>
-    </row>
-    <row r="103" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N102" s="16">
+        <v>1.8800000000000001E-2</v>
+      </c>
+    </row>
+    <row r="103" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
         <v>102</v>
       </c>
@@ -4142,8 +4379,11 @@
       <c r="M103" s="15">
         <v>1.3899999999999999E-2</v>
       </c>
-    </row>
-    <row r="104" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N103" s="16">
+        <v>1.7299999999999999E-2</v>
+      </c>
+    </row>
+    <row r="104" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
         <v>103</v>
       </c>
@@ -4171,8 +4411,11 @@
       <c r="M104" s="15">
         <v>1.37E-2</v>
       </c>
-    </row>
-    <row r="105" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N104" s="16">
+        <v>4.4000000000000003E-3</v>
+      </c>
+    </row>
+    <row r="105" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
         <v>104</v>
       </c>
@@ -4200,8 +4443,11 @@
       <c r="M105" s="15">
         <v>1.6199999999999999E-2</v>
       </c>
-    </row>
-    <row r="106" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N105" s="16">
+        <v>-3.7000000000000002E-3</v>
+      </c>
+    </row>
+    <row r="106" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
         <v>105</v>
       </c>
@@ -4229,8 +4475,11 @@
       <c r="M106" s="15">
         <v>7.7999999999999996E-3</v>
       </c>
-    </row>
-    <row r="107" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N106" s="16">
+        <v>1.4E-2</v>
+      </c>
+    </row>
+    <row r="107" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
         <v>106</v>
       </c>
@@ -4258,8 +4507,11 @@
       <c r="M107" s="15">
         <v>6.6E-3</v>
       </c>
-    </row>
-    <row r="108" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N107" s="16">
+        <v>1.23E-2</v>
+      </c>
+    </row>
+    <row r="108" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
         <v>107</v>
       </c>
@@ -4287,8 +4539,11 @@
       <c r="M108" s="15">
         <v>2.1000000000000001E-2</v>
       </c>
-    </row>
-    <row r="109" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N108" s="16">
+        <v>1.2699999999999999E-2</v>
+      </c>
+    </row>
+    <row r="109" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
         <v>108</v>
       </c>
@@ -4316,8 +4571,11 @@
       <c r="M109" s="15">
         <v>1.6000000000000001E-3</v>
       </c>
-    </row>
-    <row r="110" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N109" s="16">
+        <v>1.4E-2</v>
+      </c>
+    </row>
+    <row r="110" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
         <v>109</v>
       </c>
@@ -4345,8 +4603,11 @@
       <c r="M110" s="15">
         <v>9.4999999999999998E-3</v>
       </c>
-    </row>
-    <row r="111" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N110" s="16">
+        <v>6.6E-3</v>
+      </c>
+    </row>
+    <row r="111" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
         <v>110</v>
       </c>
@@ -4374,8 +4635,11 @@
       <c r="M111" s="15">
         <v>1.2E-2</v>
       </c>
-    </row>
-    <row r="112" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N111" s="16">
+        <v>1.01E-2</v>
+      </c>
+    </row>
+    <row r="112" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
         <v>111</v>
       </c>
@@ -4403,8 +4667,11 @@
       <c r="M112" s="15">
         <v>1.1999999999999999E-3</v>
       </c>
-    </row>
-    <row r="113" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N112" s="16">
+        <v>1.11E-2</v>
+      </c>
+    </row>
+    <row r="113" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
         <v>112</v>
       </c>
@@ -4432,8 +4699,11 @@
       <c r="M113" s="15">
         <v>4.3E-3</v>
       </c>
-    </row>
-    <row r="114" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N113" s="16">
+        <v>5.8999999999999999E-3</v>
+      </c>
+    </row>
+    <row r="114" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="s">
         <v>113</v>
       </c>
@@ -4461,8 +4731,11 @@
       <c r="M114" s="15">
         <v>9.5999999999999992E-3</v>
       </c>
-    </row>
-    <row r="115" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N114" s="16">
+        <v>6.7999999999999996E-3</v>
+      </c>
+    </row>
+    <row r="115" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
         <v>114</v>
       </c>
@@ -4490,8 +4763,11 @@
       <c r="M115" s="15">
         <v>1.49E-2</v>
       </c>
-    </row>
-    <row r="116" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N115" s="16">
+        <v>1.4E-2</v>
+      </c>
+    </row>
+    <row r="116" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
         <v>115</v>
       </c>
@@ -4519,8 +4795,11 @@
       <c r="M116" s="15">
         <v>1.54E-2</v>
       </c>
-    </row>
-    <row r="117" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N116" s="16">
+        <v>1.7100000000000001E-2</v>
+      </c>
+    </row>
+    <row r="117" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A117" s="1" t="s">
         <v>116</v>
       </c>
@@ -4548,8 +4827,11 @@
       <c r="M117" s="15">
         <v>2.1700000000000001E-2</v>
       </c>
-    </row>
-    <row r="118" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N117" s="16">
+        <v>1.61E-2</v>
+      </c>
+    </row>
+    <row r="118" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
         <v>117</v>
       </c>
@@ -4577,8 +4859,11 @@
       <c r="M118" s="15">
         <v>2.0999999999999999E-3</v>
       </c>
-    </row>
-    <row r="119" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N118" s="16">
+        <v>1.14E-2</v>
+      </c>
+    </row>
+    <row r="119" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A119" s="1" t="s">
         <v>118</v>
       </c>
@@ -4606,8 +4891,11 @@
       <c r="M119" s="15">
         <v>2.18E-2</v>
       </c>
-    </row>
-    <row r="120" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N119" s="16">
+        <v>1.11E-2</v>
+      </c>
+    </row>
+    <row r="120" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A120" s="1" t="s">
         <v>119</v>
       </c>
@@ -4635,8 +4923,11 @@
       <c r="M120" s="15">
         <v>1.3599999999999999E-2</v>
       </c>
-    </row>
-    <row r="121" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N120" s="16">
+        <v>1.1900000000000001E-2</v>
+      </c>
+    </row>
+    <row r="121" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A121" s="1" t="s">
         <v>120</v>
       </c>
@@ -4664,8 +4955,11 @@
       <c r="M121" s="15">
         <v>5.3E-3</v>
       </c>
-    </row>
-    <row r="122" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N121" s="16">
+        <v>8.9999999999999998E-4</v>
+      </c>
+    </row>
+    <row r="122" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A122" s="1" t="s">
         <v>121</v>
       </c>
@@ -4693,8 +4987,11 @@
       <c r="M122" s="15">
         <v>6.7000000000000002E-3</v>
       </c>
-    </row>
-    <row r="123" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N122" s="16">
+        <v>4.1000000000000003E-3</v>
+      </c>
+    </row>
+    <row r="123" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A123" s="1" t="s">
         <v>122</v>
       </c>
@@ -4722,8 +5019,11 @@
       <c r="M123" s="15">
         <v>5.4000000000000003E-3</v>
       </c>
-    </row>
-    <row r="124" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N123" s="16">
+        <v>1.9099999999999999E-2</v>
+      </c>
+    </row>
+    <row r="124" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A124" s="1" t="s">
         <v>123</v>
       </c>
@@ -4751,8 +5051,11 @@
       <c r="M124" s="15">
         <v>7.6E-3</v>
       </c>
-    </row>
-    <row r="125" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N124" s="16">
+        <v>1.52E-2</v>
+      </c>
+    </row>
+    <row r="125" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A125" s="1" t="s">
         <v>124</v>
       </c>
@@ -4780,8 +5083,11 @@
       <c r="M125" s="15">
         <v>1.26E-2</v>
       </c>
-    </row>
-    <row r="126" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N125" s="16">
+        <v>1.5800000000000002E-2</v>
+      </c>
+    </row>
+    <row r="126" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A126" s="1" t="s">
         <v>125</v>
       </c>
@@ -4809,8 +5115,11 @@
       <c r="M126" s="15">
         <v>6.6E-3</v>
       </c>
-    </row>
-    <row r="127" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N126" s="16">
+        <v>1.35E-2</v>
+      </c>
+    </row>
+    <row r="127" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A127" s="1" t="s">
         <v>126</v>
       </c>
@@ -4838,8 +5147,11 @@
       <c r="M127" s="15">
         <v>4.7999999999999996E-3</v>
       </c>
-    </row>
-    <row r="128" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N127" s="16">
+        <v>4.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="128" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A128" s="1" t="s">
         <v>127</v>
       </c>
@@ -4867,8 +5179,11 @@
       <c r="M128" s="15">
         <v>1.6899999999999998E-2</v>
       </c>
-    </row>
-    <row r="129" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N128" s="16">
+        <v>2.2000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="129" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A129" s="1" t="s">
         <v>128</v>
       </c>
@@ -4896,8 +5211,11 @@
       <c r="M129" s="15">
         <v>-2.7000000000000001E-3</v>
       </c>
-    </row>
-    <row r="130" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N129" s="16">
+        <v>4.8999999999999998E-3</v>
+      </c>
+    </row>
+    <row r="130" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A130" s="1" t="s">
         <v>129</v>
       </c>
@@ -4925,8 +5243,11 @@
       <c r="M130" s="15">
         <v>-1.67E-2</v>
       </c>
-    </row>
-    <row r="131" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N130" s="16">
+        <v>-3.1899999999999998E-2</v>
+      </c>
+    </row>
+    <row r="131" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A131" s="1" t="s">
         <v>130</v>
       </c>
@@ -4954,8 +5275,11 @@
       <c r="M131" s="15">
         <v>8.0999999999999996E-3</v>
       </c>
-    </row>
-    <row r="132" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N131" s="16">
+        <v>-1.0699999999999999E-2</v>
+      </c>
+    </row>
+    <row r="132" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A132" s="1" t="s">
         <v>131</v>
       </c>
@@ -4983,8 +5307,11 @@
       <c r="M132" s="15">
         <v>-6.1000000000000004E-3</v>
       </c>
-    </row>
-    <row r="133" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N132" s="16">
+        <v>-4.7999999999999996E-3</v>
+      </c>
+    </row>
+    <row r="133" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A133" s="1" t="s">
         <v>132</v>
       </c>
@@ -5012,8 +5339,11 @@
       <c r="M133" s="15">
         <v>8.5000000000000006E-3</v>
       </c>
-    </row>
-    <row r="134" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N133" s="16">
+        <v>3.3300000000000003E-2</v>
+      </c>
+    </row>
+    <row r="134" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A134" s="1" t="s">
         <v>133</v>
       </c>
@@ -5041,8 +5371,11 @@
       <c r="M134" s="15">
         <v>3.5900000000000001E-2</v>
       </c>
-    </row>
-    <row r="135" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N134" s="16">
+        <v>1.6E-2</v>
+      </c>
+    </row>
+    <row r="135" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A135" s="1" t="s">
         <v>134</v>
       </c>
@@ -5070,8 +5403,11 @@
       <c r="M135" s="15">
         <v>1.5E-3</v>
       </c>
-    </row>
-    <row r="136" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N135" s="16">
+        <v>2.1100000000000001E-2</v>
+      </c>
+    </row>
+    <row r="136" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A136" s="1" t="s">
         <v>135</v>
       </c>
@@ -5099,8 +5435,11 @@
       <c r="M136" s="15">
         <v>-1.3299999999999999E-2</v>
       </c>
-    </row>
-    <row r="137" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N136" s="16">
+        <v>2.5000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="137" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A137" s="1" t="s">
         <v>136</v>
       </c>
@@ -5128,8 +5467,11 @@
       <c r="M137" s="15">
         <v>-7.6E-3</v>
       </c>
-    </row>
-    <row r="138" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N137" s="16">
+        <v>1.5299999999999999E-2</v>
+      </c>
+    </row>
+    <row r="138" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A138" s="1" t="s">
         <v>137</v>
       </c>
@@ -5157,8 +5499,11 @@
       <c r="M138" s="15">
         <v>-6.4999999999999997E-3</v>
       </c>
-    </row>
-    <row r="139" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N138" s="16">
+        <v>2.6599999999999999E-2</v>
+      </c>
+    </row>
+    <row r="139" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A139" s="1" t="s">
         <v>138</v>
       </c>
@@ -5186,8 +5531,11 @@
       <c r="M139" s="15">
         <v>1.6999999999999999E-3</v>
       </c>
-    </row>
-    <row r="140" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N139" s="16">
+        <v>1.4E-2</v>
+      </c>
+    </row>
+    <row r="140" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A140" s="1" t="s">
         <v>139</v>
       </c>
@@ -5215,8 +5563,11 @@
       <c r="M140" s="15">
         <v>2.0199999999999999E-2</v>
       </c>
-    </row>
-    <row r="141" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N140" s="16">
+        <v>1.09E-2</v>
+      </c>
+    </row>
+    <row r="141" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A141" s="1" t="s">
         <v>140</v>
       </c>
@@ -5244,8 +5595,11 @@
       <c r="M141" s="15">
         <v>1.9099999999999999E-2</v>
       </c>
-    </row>
-    <row r="142" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N141" s="16">
+        <v>1.0500000000000001E-2</v>
+      </c>
+    </row>
+    <row r="142" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A142" s="1" t="s">
         <v>141</v>
       </c>
@@ -5273,8 +5627,11 @@
       <c r="M142" s="15">
         <v>7.0000000000000001E-3</v>
       </c>
-    </row>
-    <row r="143" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N142" s="16">
+        <v>4.1999999999999997E-3</v>
+      </c>
+    </row>
+    <row r="143" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A143" s="1" t="s">
         <v>142</v>
       </c>
@@ -5302,8 +5659,11 @@
       <c r="M143" s="15">
         <v>8.5000000000000006E-3</v>
       </c>
-    </row>
-    <row r="144" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N143" s="16">
+        <v>6.6E-3</v>
+      </c>
+    </row>
+    <row r="144" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A144" s="1" t="s">
         <v>143</v>
       </c>
@@ -5331,8 +5691,11 @@
       <c r="M144" s="15">
         <v>4.4000000000000003E-3</v>
       </c>
-    </row>
-    <row r="145" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N144" s="16">
+        <v>3.3E-3</v>
+      </c>
+    </row>
+    <row r="145" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A145" s="1" t="s">
         <v>144</v>
       </c>
@@ -5360,8 +5723,11 @@
       <c r="M145" s="15">
         <v>1.0500000000000001E-2</v>
       </c>
-    </row>
-    <row r="146" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N145" s="16">
+        <v>9.9000000000000008E-3</v>
+      </c>
+    </row>
+    <row r="146" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A146" s="1" t="s">
         <v>145</v>
       </c>
@@ -5389,8 +5755,11 @@
       <c r="M146" s="15">
         <v>2.3900000000000001E-2</v>
       </c>
-    </row>
-    <row r="147" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N146" s="16">
+        <v>1.0800000000000001E-2</v>
+      </c>
+    </row>
+    <row r="147" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A147" s="1" t="s">
         <v>146</v>
       </c>
@@ -5418,8 +5787,11 @@
       <c r="M147" s="15">
         <v>-1.1900000000000001E-2</v>
       </c>
-    </row>
-    <row r="148" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N147" s="16">
+        <v>1.9099999999999999E-2</v>
+      </c>
+    </row>
+    <row r="148" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A148" s="1" t="s">
         <v>147</v>
       </c>
@@ -5447,8 +5819,11 @@
       <c r="M148" s="15">
         <v>2.2599999999999999E-2</v>
       </c>
-    </row>
-    <row r="149" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N148" s="16">
+        <v>2.2100000000000002E-2</v>
+      </c>
+    </row>
+    <row r="149" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A149" s="1" t="s">
         <v>148</v>
       </c>
@@ -5476,8 +5851,11 @@
       <c r="M149" s="15">
         <v>4.7999999999999996E-3</v>
       </c>
-    </row>
-    <row r="150" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N149" s="16">
+        <v>1.7500000000000002E-2</v>
+      </c>
+    </row>
+    <row r="150" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A150" s="1" t="s">
         <v>149</v>
       </c>
@@ -5505,8 +5883,11 @@
       <c r="M150" s="15">
         <v>2.64E-2</v>
       </c>
-    </row>
-    <row r="151" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N150" s="16">
+        <v>1.78E-2</v>
+      </c>
+    </row>
+    <row r="151" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A151" s="1" t="s">
         <v>150</v>
       </c>
@@ -5534,8 +5915,11 @@
       <c r="M151" s="15">
         <v>2.7000000000000001E-3</v>
       </c>
-    </row>
-    <row r="152" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N151" s="16">
+        <v>1.34E-2</v>
+      </c>
+    </row>
+    <row r="152" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A152" s="1" t="s">
         <v>151</v>
       </c>
@@ -5563,8 +5947,11 @@
       <c r="M152" s="15">
         <v>1.4999999999999999E-2</v>
       </c>
-    </row>
-    <row r="153" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N152" s="16">
+        <v>1.66E-2</v>
+      </c>
+    </row>
+    <row r="153" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A153" s="1" t="s">
         <v>152</v>
       </c>
@@ -5592,8 +5979,11 @@
       <c r="M153" s="15">
         <v>-4.0000000000000002E-4</v>
       </c>
-    </row>
-    <row r="154" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N153" s="16">
+        <v>6.7999999999999996E-3</v>
+      </c>
+    </row>
+    <row r="154" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A154" s="1" t="s">
         <v>153</v>
       </c>
@@ -5621,8 +6011,11 @@
       <c r="M154" s="15">
         <v>3.0599999999999999E-2</v>
       </c>
-    </row>
-    <row r="155" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N154" s="16">
+        <v>1.4200000000000001E-2</v>
+      </c>
+    </row>
+    <row r="155" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A155" s="1" t="s">
         <v>154</v>
       </c>
@@ -5650,8 +6043,11 @@
       <c r="M155" s="15">
         <v>9.4000000000000004E-3</v>
       </c>
-    </row>
-    <row r="156" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N155" s="16">
+        <v>1.21E-2</v>
+      </c>
+    </row>
+    <row r="156" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A156" s="1" t="s">
         <v>155</v>
       </c>
@@ -5679,8 +6075,11 @@
       <c r="M156" s="15">
         <v>2.3E-3</v>
       </c>
-    </row>
-    <row r="157" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N156" s="16">
+        <v>4.1999999999999997E-3</v>
+      </c>
+    </row>
+    <row r="157" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A157" s="1" t="s">
         <v>156</v>
       </c>
@@ -5708,8 +6107,11 @@
       <c r="M157" s="15">
         <v>1.03E-2</v>
       </c>
-    </row>
-    <row r="158" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N157" s="16">
+        <v>-7.1000000000000004E-3</v>
+      </c>
+    </row>
+    <row r="158" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A158" s="1" t="s">
         <v>157</v>
       </c>
@@ -5737,8 +6139,11 @@
       <c r="M158" s="15">
         <v>2.58E-2</v>
       </c>
-    </row>
-    <row r="159" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N158" s="16">
+        <v>-1E-4</v>
+      </c>
+    </row>
+    <row r="159" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A159" s="1" t="s">
         <v>158</v>
       </c>
@@ -5766,8 +6171,11 @@
       <c r="M159" s="15">
         <v>-1.5699999999999999E-2</v>
       </c>
-    </row>
-    <row r="160" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N159" s="16">
+        <v>2.7300000000000001E-2</v>
+      </c>
+    </row>
+    <row r="160" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A160" s="1" t="s">
         <v>159</v>
       </c>
@@ -5795,8 +6203,11 @@
       <c r="M160" s="15">
         <v>2.07E-2</v>
       </c>
-    </row>
-    <row r="161" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N160" s="16">
+        <v>1.7000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="161" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A161" s="1" t="s">
         <v>160</v>
       </c>
@@ -5824,8 +6235,11 @@
       <c r="M161" s="15">
         <v>1.77E-2</v>
       </c>
-    </row>
-    <row r="162" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N161" s="16">
+        <v>1.6799999999999999E-2</v>
+      </c>
+    </row>
+    <row r="162" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A162" s="1" t="s">
         <v>161</v>
       </c>
@@ -5853,8 +6267,11 @@
       <c r="M162" s="15">
         <v>5.9999999999999995E-4</v>
       </c>
-    </row>
-    <row r="163" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N162" s="16">
+        <v>1.5699999999999999E-2</v>
+      </c>
+    </row>
+    <row r="163" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A163" s="1" t="s">
         <v>162</v>
       </c>
@@ -5882,8 +6299,11 @@
       <c r="M163" s="15">
         <v>2.8E-3</v>
       </c>
-    </row>
-    <row r="164" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N163" s="16">
+        <v>7.1000000000000004E-3</v>
+      </c>
+    </row>
+    <row r="164" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A164" s="1" t="s">
         <v>163</v>
       </c>
@@ -5911,8 +6331,11 @@
       <c r="M164" s="15">
         <v>3.5999999999999999E-3</v>
       </c>
-    </row>
-    <row r="165" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N164" s="16">
+        <v>1.2999999999999999E-3</v>
+      </c>
+    </row>
+    <row r="165" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A165" s="1" t="s">
         <v>164</v>
       </c>
@@ -5940,8 +6363,11 @@
       <c r="M165" s="15">
         <v>4.4999999999999997E-3</v>
       </c>
-    </row>
-    <row r="166" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N165" s="16">
+        <v>7.6E-3</v>
+      </c>
+    </row>
+    <row r="166" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A166" s="1" t="s">
         <v>165</v>
       </c>
@@ -5969,8 +6395,11 @@
       <c r="M166" s="15">
         <v>1.7299999999999999E-2</v>
       </c>
-    </row>
-    <row r="167" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N166" s="16">
+        <v>1.26E-2</v>
+      </c>
+    </row>
+    <row r="167" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A167" s="1" t="s">
         <v>166</v>
       </c>
@@ -5998,8 +6427,11 @@
       <c r="M167" s="15">
         <v>1.3100000000000001E-2</v>
       </c>
-    </row>
-    <row r="168" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N167" s="16">
+        <v>6.4000000000000003E-3</v>
+      </c>
+    </row>
+    <row r="168" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A168" s="1" t="s">
         <v>167</v>
       </c>
@@ -6027,8 +6459,11 @@
       <c r="M168" s="15">
         <v>1E-4</v>
       </c>
-    </row>
-    <row r="169" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N168" s="16">
+        <v>9.2999999999999992E-3</v>
+      </c>
+    </row>
+    <row r="169" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A169" s="1" t="s">
         <v>168</v>
       </c>
@@ -6056,8 +6491,11 @@
       <c r="M169" s="15">
         <v>-3.5999999999999999E-3</v>
       </c>
-    </row>
-    <row r="170" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N169" s="16">
+        <v>6.1999999999999998E-3</v>
+      </c>
+    </row>
+    <row r="170" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A170" s="1" t="s">
         <v>169</v>
       </c>
@@ -6085,8 +6523,11 @@
       <c r="M170" s="15">
         <v>4.5999999999999999E-3</v>
       </c>
-    </row>
-    <row r="171" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N170" s="16">
+        <v>-8.0000000000000004E-4</v>
+      </c>
+    </row>
+    <row r="171" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A171" s="1" t="s">
         <v>170</v>
       </c>
@@ -6114,8 +6555,11 @@
       <c r="M171" s="15">
         <v>7.6140000000000001E-3</v>
       </c>
-    </row>
-    <row r="172" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N171" s="16">
+        <v>1.3845E-2</v>
+      </c>
+    </row>
+    <row r="172" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A172" s="1" t="s">
         <v>171</v>
       </c>
@@ -6143,8 +6587,11 @@
       <c r="M172" s="15">
         <v>-2.2200000000000002E-3</v>
       </c>
-    </row>
-    <row r="173" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N172" s="16">
+        <v>1.8630000000000001E-3</v>
+      </c>
+    </row>
+    <row r="173" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A173" s="1" t="s">
         <v>172</v>
       </c>
@@ -6172,8 +6619,11 @@
       <c r="M173" s="15">
         <v>5.53E-4</v>
       </c>
-    </row>
-    <row r="174" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N173" s="16">
+        <v>4.6109999999999996E-3</v>
+      </c>
+    </row>
+    <row r="174" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A174" s="1" t="s">
         <v>173</v>
       </c>
@@ -6201,8 +6651,11 @@
       <c r="M174" s="15">
         <v>9.9139999999999992E-3</v>
       </c>
-    </row>
-    <row r="175" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N174" s="16">
+        <v>8.659E-3</v>
+      </c>
+    </row>
+    <row r="175" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A175" s="1" t="s">
         <v>174</v>
       </c>
@@ -6230,8 +6683,11 @@
       <c r="M175" s="15">
         <v>3.1300000000000002E-4</v>
       </c>
-    </row>
-    <row r="176" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N175" s="16">
+        <v>5.2659999999999998E-3</v>
+      </c>
+    </row>
+    <row r="176" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A176" s="1" t="s">
         <v>175</v>
       </c>
@@ -6259,8 +6715,11 @@
       <c r="M176" s="15">
         <v>4.9899999999999999E-4</v>
       </c>
-    </row>
-    <row r="177" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N176" s="16">
+        <v>2.232E-3</v>
+      </c>
+    </row>
+    <row r="177" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A177" s="1" t="s">
         <v>176</v>
       </c>
@@ -6288,8 +6747,11 @@
       <c r="M177" s="15">
         <v>-2.6930000000000001E-3</v>
       </c>
-    </row>
-    <row r="178" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N177" s="16">
+        <v>-1.2813E-2</v>
+      </c>
+    </row>
+    <row r="178" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A178" s="1" t="s">
         <v>177</v>
       </c>
@@ -6317,8 +6779,11 @@
       <c r="M178" s="15">
         <v>5.3350000000000003E-3</v>
       </c>
-    </row>
-    <row r="179" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N178" s="16">
+        <v>3.5239999999999998E-3</v>
+      </c>
+    </row>
+    <row r="179" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A179" s="1" t="s">
         <v>178</v>
       </c>
@@ -6346,8 +6811,11 @@
       <c r="M179" s="15">
         <v>-2.4499999999999999E-3</v>
       </c>
-    </row>
-    <row r="180" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N179" s="16">
+        <v>1.5859999999999999E-2</v>
+      </c>
+    </row>
+    <row r="180" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A180" s="1" t="s">
         <v>179</v>
       </c>
@@ -6375,8 +6843,11 @@
       <c r="M180" s="15">
         <v>-2.905E-3</v>
       </c>
-    </row>
-    <row r="181" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N180" s="16">
+        <v>9.9670000000000002E-3</v>
+      </c>
+    </row>
+    <row r="181" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A181" s="1" t="s">
         <v>180</v>
       </c>
@@ -6404,8 +6875,11 @@
       <c r="M181" s="15">
         <v>-9.1079999999999998E-3</v>
       </c>
-    </row>
-    <row r="182" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N181" s="16">
+        <v>2.0157000000000001E-2</v>
+      </c>
+    </row>
+    <row r="182" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A182" s="1" t="s">
         <v>181</v>
       </c>
@@ -6433,8 +6907,11 @@
       <c r="M182" s="15">
         <v>5.0600000000000003E-3</v>
       </c>
-    </row>
-    <row r="183" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N182" s="16">
+        <v>1.421E-2</v>
+      </c>
+    </row>
+    <row r="183" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A183" s="1" t="s">
         <v>182</v>
       </c>
@@ -6462,8 +6939,11 @@
       <c r="M183" s="15">
         <v>2.97E-3</v>
       </c>
-    </row>
-    <row r="184" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N183" s="16">
+        <v>2.4989999999999998E-2</v>
+      </c>
+    </row>
+    <row r="184" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A184" s="1" t="s">
         <v>183</v>
       </c>
@@ -6491,8 +6971,11 @@
       <c r="M184" s="15">
         <v>-1.83E-3</v>
       </c>
-    </row>
-    <row r="185" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N184" s="16">
+        <v>1.289E-2</v>
+      </c>
+    </row>
+    <row r="185" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A185" s="1" t="s">
         <v>184</v>
       </c>
@@ -6520,8 +7003,11 @@
       <c r="M185" s="15">
         <v>-4.6999999999999999E-4</v>
       </c>
-    </row>
-    <row r="186" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N185" s="16">
+        <v>7.3000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="186" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A186" s="1" t="s">
         <v>185</v>
       </c>
@@ -6549,8 +7035,11 @@
       <c r="M186" s="15">
         <v>3.62E-3</v>
       </c>
-    </row>
-    <row r="187" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N186" s="16">
+        <v>1.359E-2</v>
+      </c>
+    </row>
+    <row r="187" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A187" s="1" t="s">
         <v>186</v>
       </c>
@@ -6578,8 +7067,11 @@
       <c r="M187" s="15">
         <v>3.5100000000000001E-3</v>
       </c>
-    </row>
-    <row r="188" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N187" s="16">
+        <v>1.1429999999999999E-2</v>
+      </c>
+    </row>
+    <row r="188" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A188" s="1" t="s">
         <v>187</v>
       </c>
@@ -6607,8 +7099,11 @@
       <c r="M188" s="15">
         <v>3.96E-3</v>
       </c>
-    </row>
-    <row r="189" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N188" s="16">
+        <v>-5.7200000000000003E-3</v>
+      </c>
+    </row>
+    <row r="189" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A189" s="1" t="s">
         <v>188</v>
       </c>
@@ -6636,8 +7131,11 @@
       <c r="M189" s="15">
         <v>-4.4200000000000003E-3</v>
       </c>
-    </row>
-    <row r="190" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N189" s="16">
+        <v>-6.9699999999999996E-3</v>
+      </c>
+    </row>
+    <row r="190" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A190" s="1" t="s">
         <v>189</v>
       </c>
@@ -6665,8 +7163,11 @@
       <c r="M190" s="15">
         <v>1.31E-3</v>
       </c>
-    </row>
-    <row r="191" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N190" s="16">
+        <v>-6.8500000000000002E-3</v>
+      </c>
+    </row>
+    <row r="191" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A191" s="1" t="s">
         <v>190</v>
       </c>
@@ -6694,8 +7195,11 @@
       <c r="M191" s="15">
         <v>5.96E-3</v>
       </c>
-    </row>
-    <row r="192" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N191" s="16">
+        <v>1.4080000000000001E-2</v>
+      </c>
+    </row>
+    <row r="192" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A192" s="1" t="s">
         <v>191</v>
       </c>
@@ -6723,8 +7227,11 @@
       <c r="M192" s="15">
         <v>1.056E-2</v>
       </c>
-    </row>
-    <row r="193" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N192" s="16">
+        <v>1.397E-2</v>
+      </c>
+    </row>
+    <row r="193" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A193" s="1" t="s">
         <v>192</v>
       </c>
@@ -6752,8 +7259,11 @@
       <c r="M193" s="15">
         <v>2.0400000000000001E-3</v>
       </c>
-    </row>
-    <row r="194" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N193" s="16">
+        <v>8.1200000000000005E-3</v>
+      </c>
+    </row>
+    <row r="194" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A194" s="1" t="s">
         <v>193</v>
       </c>
@@ -6781,8 +7291,11 @@
       <c r="M194" s="15">
         <v>-2.9399999999999999E-3</v>
       </c>
-    </row>
-    <row r="195" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N194" s="16">
+        <v>8.7899999999999992E-3</v>
+      </c>
+    </row>
+    <row r="195" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A195" s="1" t="s">
         <v>194</v>
       </c>
@@ -6810,8 +7323,11 @@
       <c r="M195" s="15">
         <v>1.074E-2</v>
       </c>
-    </row>
-    <row r="196" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N195" s="16">
+        <v>1.013E-2</v>
+      </c>
+    </row>
+    <row r="196" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A196" s="1" t="s">
         <v>195</v>
       </c>
@@ -6839,8 +7355,11 @@
       <c r="M196" s="15">
         <v>5.6699999999999997E-3</v>
       </c>
-    </row>
-    <row r="197" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N196" s="16">
+        <v>1.7700000000000001E-3</v>
+      </c>
+    </row>
+    <row r="197" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A197" s="1" t="s">
         <v>196</v>
       </c>
@@ -6868,8 +7387,11 @@
       <c r="M197" s="15">
         <v>4.0499999999999998E-3</v>
       </c>
-    </row>
-    <row r="198" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N197" s="16">
+        <v>6.77E-3</v>
+      </c>
+    </row>
+    <row r="198" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A198" s="1" t="s">
         <v>197</v>
       </c>
@@ -6897,8 +7419,11 @@
       <c r="M198" s="15">
         <v>-1.145E-2</v>
       </c>
-    </row>
-    <row r="199" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N198" s="16">
+        <v>2.5100000000000001E-3</v>
+      </c>
+    </row>
+    <row r="199" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A199" s="1" t="s">
         <v>198</v>
       </c>
@@ -6926,8 +7451,11 @@
       <c r="M199" s="15">
         <v>3.4499999999999999E-3</v>
       </c>
-    </row>
-    <row r="200" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N199" s="16">
+        <v>-1.191E-2</v>
+      </c>
+    </row>
+    <row r="200" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A200" s="1" t="s">
         <v>199</v>
       </c>
@@ -6955,8 +7483,11 @@
       <c r="M200" s="15">
         <v>3.7499999999999999E-3</v>
       </c>
-    </row>
-    <row r="201" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N200" s="16">
+        <v>-1.04E-2</v>
+      </c>
+    </row>
+    <row r="201" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A201" s="1" t="s">
         <v>200</v>
       </c>
@@ -6984,8 +7515,11 @@
       <c r="M201" s="15">
         <v>1.8400000000000001E-3</v>
       </c>
-    </row>
-    <row r="202" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N201" s="16">
+        <v>4.5900000000000003E-3</v>
+      </c>
+    </row>
+    <row r="202" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A202" s="1" t="s">
         <v>201</v>
       </c>
@@ -7013,8 +7547,11 @@
       <c r="M202" s="15">
         <v>-2.2499999999999998E-3</v>
       </c>
-    </row>
-    <row r="203" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N202" s="16">
+        <v>2.6700000000000001E-3</v>
+      </c>
+    </row>
+    <row r="203" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A203" s="1" t="s">
         <v>202</v>
       </c>
@@ -7042,8 +7579,11 @@
       <c r="M203" s="15">
         <v>7.8799999999999999E-3</v>
       </c>
-    </row>
-    <row r="204" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N203" s="16">
+        <v>-2.4499999999999999E-3</v>
+      </c>
+    </row>
+    <row r="204" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A204" s="1" t="s">
         <v>203</v>
       </c>
@@ -7071,8 +7611,11 @@
       <c r="M204" s="15">
         <v>-6.0000000000000002E-5</v>
       </c>
-    </row>
-    <row r="205" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N204" s="16">
+        <v>-4.7800000000000004E-3</v>
+      </c>
+    </row>
+    <row r="205" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A205" s="1" t="s">
         <v>204</v>
       </c>
@@ -7100,8 +7643,11 @@
       <c r="M205" s="15">
         <v>1.308E-2</v>
       </c>
-    </row>
-    <row r="206" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N205" s="16">
+        <v>8.8299999999999993E-3</v>
+      </c>
+    </row>
+    <row r="206" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A206" s="1" t="s">
         <v>205</v>
       </c>
@@ -7129,8 +7675,11 @@
       <c r="M206" s="15">
         <v>4.2500000000000003E-3</v>
       </c>
-    </row>
-    <row r="207" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N206" s="16">
+        <v>4.2900000000000004E-3</v>
+      </c>
+    </row>
+    <row r="207" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A207" s="1" t="s">
         <v>206</v>
       </c>
@@ -7158,8 +7707,11 @@
       <c r="M207" s="15">
         <v>6.3600000000000002E-3</v>
       </c>
-    </row>
-    <row r="208" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N207" s="16">
+        <v>-9.0100000000000006E-3</v>
+      </c>
+    </row>
+    <row r="208" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A208" s="1" t="s">
         <v>207</v>
       </c>
@@ -7187,8 +7739,11 @@
       <c r="M208" s="15">
         <v>1.1610000000000001E-2</v>
       </c>
-    </row>
-    <row r="209" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N208" s="16">
+        <v>-4.4299999999999999E-3</v>
+      </c>
+    </row>
+    <row r="209" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A209" s="1" t="s">
         <v>208</v>
       </c>
@@ -7216,8 +7771,11 @@
       <c r="M209" s="15">
         <v>9.6000000000000002E-4</v>
       </c>
-    </row>
-    <row r="210" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N209" s="16">
+        <v>-1.4789999999999999E-2</v>
+      </c>
+    </row>
+    <row r="210" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A210" s="1" t="s">
         <v>209</v>
       </c>
@@ -7245,8 +7803,11 @@
       <c r="M210" s="15">
         <v>-3.8300000000000001E-3</v>
       </c>
-    </row>
-    <row r="211" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N210" s="16">
+        <v>-2.64E-2</v>
+      </c>
+    </row>
+    <row r="211" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A211" s="1" t="s">
         <v>210</v>
       </c>
@@ -7274,8 +7835,11 @@
       <c r="M211" s="15">
         <v>5.7600000000000004E-3</v>
       </c>
-    </row>
-    <row r="212" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N211" s="16">
+        <v>-1.1679999999999999E-2</v>
+      </c>
+    </row>
+    <row r="212" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A212" s="1" t="s">
         <v>211</v>
       </c>
@@ -7303,8 +7867,11 @@
       <c r="M212" s="15">
         <v>8.3899999999999999E-3</v>
       </c>
-    </row>
-    <row r="213" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N212" s="16">
+        <v>1.0290000000000001E-2</v>
+      </c>
+    </row>
+    <row r="213" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A213" s="1" t="s">
         <v>212</v>
       </c>
@@ -7332,8 +7899,11 @@
       <c r="M213" s="15">
         <v>8.1600000000000006E-3</v>
       </c>
-    </row>
-    <row r="214" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N213" s="16">
+        <v>1.0840000000000001E-2</v>
+      </c>
+    </row>
+    <row r="214" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A214" s="1" t="s">
         <v>213</v>
       </c>
@@ -7361,8 +7931,11 @@
       <c r="M214" s="15">
         <v>5.62E-3</v>
       </c>
-    </row>
-    <row r="215" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N214" s="16">
+        <v>5.7999999999999996E-3</v>
+      </c>
+    </row>
+    <row r="215" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A215" s="1" t="s">
         <v>214</v>
       </c>
@@ -7390,8 +7963,11 @@
       <c r="M215" s="15">
         <v>9.5200000000000007E-3</v>
       </c>
-    </row>
-    <row r="216" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N215" s="16">
+        <v>1.265E-2</v>
+      </c>
+    </row>
+    <row r="216" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A216" s="1" t="s">
         <v>215</v>
       </c>
@@ -7419,8 +7995,11 @@
       <c r="M216" s="15">
         <v>-2.97E-3</v>
       </c>
-    </row>
-    <row r="217" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N216" s="16">
+        <v>-7.3999999999999999E-4</v>
+      </c>
+    </row>
+    <row r="217" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A217" s="1" t="s">
         <v>216</v>
       </c>
@@ -7448,8 +8027,11 @@
       <c r="M217" s="15">
         <v>5.6299999999999996E-3</v>
       </c>
-    </row>
-    <row r="218" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N217" s="16">
+        <v>4.0999999999999999E-4</v>
+      </c>
+    </row>
+    <row r="218" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A218" s="1" t="s">
         <v>217</v>
       </c>
@@ -7477,8 +8059,11 @@
       <c r="M218" s="15">
         <v>5.4400000000000004E-3</v>
       </c>
-    </row>
-    <row r="219" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N218" s="16">
+        <v>9.0799999999999995E-3</v>
+      </c>
+    </row>
+    <row r="219" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A219" s="1" t="s">
         <v>218</v>
       </c>
@@ -7506,8 +8091,11 @@
       <c r="M219" s="15">
         <v>1.452E-2</v>
       </c>
-    </row>
-    <row r="220" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N219" s="16">
+        <v>2.4029999999999999E-2</v>
+      </c>
+    </row>
+    <row r="220" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A220" s="1" t="s">
         <v>219</v>
       </c>
@@ -7535,8 +8123,11 @@
       <c r="M220" s="15">
         <v>2.7399999999999998E-3</v>
       </c>
-    </row>
-    <row r="221" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N220" s="16">
+        <v>1.166E-2</v>
+      </c>
+    </row>
+    <row r="221" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A221" s="1" t="s">
         <v>220</v>
       </c>
@@ -7564,8 +8155,11 @@
       <c r="M221" s="15">
         <v>9.11E-3</v>
       </c>
-    </row>
-    <row r="222" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N221" s="16">
+        <v>1.038E-2</v>
+      </c>
+    </row>
+    <row r="222" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A222" s="1" t="s">
         <v>221</v>
       </c>
@@ -7593,8 +8187,11 @@
       <c r="M222" s="15">
         <v>1.289E-2</v>
       </c>
-    </row>
-    <row r="223" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N222" s="16">
+        <v>6.4200000000000004E-3</v>
+      </c>
+    </row>
+    <row r="223" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A223" s="1" t="s">
         <v>222</v>
       </c>
@@ -7622,8 +8219,11 @@
       <c r="M223" s="15">
         <v>-7.1000000000000002E-4</v>
       </c>
-    </row>
-    <row r="224" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N223" s="16">
+        <v>7.8899999999999994E-3</v>
+      </c>
+    </row>
+    <row r="224" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A224" s="1" t="s">
         <v>223</v>
       </c>
@@ -7651,8 +8251,11 @@
       <c r="M224" s="15">
         <v>6.2700000000000004E-3</v>
       </c>
-    </row>
-    <row r="225" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N224" s="16">
+        <v>1.0200000000000001E-3</v>
+      </c>
+    </row>
+    <row r="225" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A225" s="1" t="s">
         <v>224</v>
       </c>
@@ -7680,8 +8283,11 @@
       <c r="M225" s="15">
         <v>3.63E-3</v>
       </c>
-    </row>
-    <row r="226" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N225" s="16">
+        <v>7.2700000000000004E-3</v>
+      </c>
+    </row>
+    <row r="226" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A226" s="1" t="s">
         <v>225</v>
       </c>
@@ -7709,8 +8315,11 @@
       <c r="M226" s="15">
         <v>5.9000000000000003E-4</v>
       </c>
-    </row>
-    <row r="227" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N226" s="16">
+        <v>1.107E-2</v>
+      </c>
+    </row>
+    <row r="227" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A227" s="1" t="s">
         <v>226</v>
       </c>
@@ -7738,8 +8347,11 @@
       <c r="M227" s="15">
         <v>2.1099999999999999E-3</v>
       </c>
-    </row>
-    <row r="228" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N227" s="16">
+        <v>9.0900000000000009E-3</v>
+      </c>
+    </row>
+    <row r="228" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A228" s="1" t="s">
         <v>227</v>
       </c>
@@ -7767,8 +8379,11 @@
       <c r="M228" s="15">
         <v>6.7299999999999999E-3</v>
       </c>
-    </row>
-    <row r="229" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N228" s="16">
+        <v>3.3999999999999998E-3</v>
+      </c>
+    </row>
+    <row r="229" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A229" s="1" t="s">
         <v>228</v>
       </c>
@@ -7796,8 +8411,11 @@
       <c r="M229" s="15">
         <v>4.8500000000000001E-3</v>
       </c>
-    </row>
-    <row r="230" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N229" s="16">
+        <v>1.112E-2</v>
+      </c>
+    </row>
+    <row r="230" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A230" s="1" t="s">
         <v>229</v>
       </c>
@@ -7825,8 +8443,11 @@
       <c r="M230" s="15">
         <v>8.2500000000000004E-3</v>
       </c>
-    </row>
-    <row r="231" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N230" s="16">
+        <v>1.221E-2</v>
+      </c>
+    </row>
+    <row r="231" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A231" s="1" t="s">
         <v>230</v>
       </c>
@@ -7854,8 +8475,11 @@
       <c r="M231" s="15">
         <v>8.3940000000000004E-3</v>
       </c>
-    </row>
-    <row r="232" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N231" s="16">
+        <v>1.3351E-2</v>
+      </c>
+    </row>
+    <row r="232" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A232" s="1" t="s">
         <v>231</v>
       </c>
@@ -7883,8 +8507,11 @@
       <c r="M232" s="15">
         <v>2.3500000000000001E-3</v>
       </c>
-    </row>
-    <row r="233" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N232" s="16">
+        <v>1.0473E-2</v>
+      </c>
+    </row>
+    <row r="233" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A233" s="1" t="s">
         <v>232</v>
       </c>
@@ -7912,8 +8539,11 @@
       <c r="M233" s="15">
         <v>9.2060000000000006E-3</v>
       </c>
-    </row>
-    <row r="234" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N233" s="16">
+        <v>4.6369999999999996E-3</v>
+      </c>
+    </row>
+    <row r="234" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A234" s="1" t="s">
         <v>233</v>
       </c>
@@ -7941,8 +8571,11 @@
       <c r="M234" s="15">
         <v>7.6610000000000003E-3</v>
       </c>
-    </row>
-    <row r="235" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N234" s="16">
+        <v>3.4220000000000001E-3</v>
+      </c>
+    </row>
+    <row r="235" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A235" s="1" t="s">
         <v>234</v>
       </c>
@@ -7970,8 +8603,11 @@
       <c r="M235" s="15">
         <v>1.2612999999999999E-2</v>
       </c>
-    </row>
-    <row r="236" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N235" s="16">
+        <v>1.2553999999999999E-2</v>
+      </c>
+    </row>
+    <row r="236" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A236" s="1" t="s">
         <v>235</v>
       </c>
@@ -7999,8 +8635,11 @@
       <c r="M236" s="15">
         <v>7.0780000000000001E-3</v>
       </c>
-    </row>
-    <row r="237" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N236" s="16">
+        <v>1.114E-3</v>
+      </c>
+    </row>
+    <row r="237" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A237" s="1" t="s">
         <v>236</v>
       </c>
@@ -8031,8 +8670,11 @@
       <c r="M237" s="15">
         <v>-4.8200000000000001E-4</v>
       </c>
-    </row>
-    <row r="238" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N237" s="16">
+        <v>-4.7540000000000004E-3</v>
+      </c>
+    </row>
+    <row r="238" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A238" s="1" t="s">
         <v>237</v>
       </c>
@@ -8063,8 +8705,11 @@
       <c r="M238" s="15">
         <v>-1.2585000000000001E-2</v>
       </c>
-    </row>
-    <row r="239" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N238" s="16">
+        <v>-1.0189999999999999E-2</v>
+      </c>
+    </row>
+    <row r="239" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A239" s="1" t="s">
         <v>238</v>
       </c>
@@ -8095,8 +8740,11 @@
       <c r="M239" s="15">
         <v>7.2040000000000003E-3</v>
       </c>
-    </row>
-    <row r="240" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N239" s="16">
+        <v>1.5722E-2</v>
+      </c>
+    </row>
+    <row r="240" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A240" s="1" t="s">
         <v>239</v>
       </c>
@@ -8127,8 +8775,11 @@
       <c r="M240" s="15">
         <v>8.9980000000000008E-3</v>
       </c>
-    </row>
-    <row r="241" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N240" s="16">
+        <v>1.9612000000000001E-2</v>
+      </c>
+    </row>
+    <row r="241" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A241" s="1" t="s">
         <v>240</v>
       </c>
@@ -8159,8 +8810,11 @@
       <c r="M241" s="15">
         <v>-2.9529999999999999E-3</v>
       </c>
-    </row>
-    <row r="242" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N241" s="16">
+        <v>-1.0336E-2</v>
+      </c>
+    </row>
+    <row r="242" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A242" s="1" t="s">
         <v>241</v>
       </c>
@@ -8191,8 +8845,11 @@
       <c r="M242" s="15">
         <v>4.4809999999999997E-3</v>
       </c>
-    </row>
-    <row r="243" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N242" s="16">
+        <v>-3.0379999999999999E-3</v>
+      </c>
+    </row>
+    <row r="243" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A243" s="1" t="s">
         <v>242</v>
       </c>
@@ -8232,8 +8889,11 @@
       <c r="M243" s="15">
         <v>-1.0368E-2</v>
       </c>
-    </row>
-    <row r="244" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N243" s="16">
+        <v>-1.3972999999999999E-2</v>
+      </c>
+    </row>
+    <row r="244" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A244" s="1" t="s">
         <v>243</v>
       </c>
@@ -8273,8 +8933,11 @@
       <c r="M244" s="15">
         <v>1.4456E-2</v>
       </c>
-    </row>
-    <row r="245" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N244" s="16">
+        <v>-7.783E-3</v>
+      </c>
+    </row>
+    <row r="245" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A245" s="1" t="s">
         <v>244</v>
       </c>
@@ -8314,8 +8977,11 @@
       <c r="M245" s="15">
         <v>-5.6750000000000004E-3</v>
       </c>
-    </row>
-    <row r="246" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N245" s="16">
+        <v>-4.1631000000000001E-2</v>
+      </c>
+    </row>
+    <row r="246" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A246" s="1" t="s">
         <v>245</v>
       </c>
@@ -8355,8 +9021,11 @@
       <c r="M246" s="15">
         <v>1.619E-3</v>
       </c>
-    </row>
-    <row r="247" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N246" s="16">
+        <v>1.3077E-2</v>
+      </c>
+    </row>
+    <row r="247" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A247" s="1" t="s">
         <v>246</v>
       </c>
@@ -8396,8 +9065,11 @@
       <c r="M247" s="15">
         <v>1.1216E-2</v>
       </c>
-    </row>
-    <row r="248" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N247" s="16">
+        <v>7.7190000000000002E-3</v>
+      </c>
+    </row>
+    <row r="248" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A248" s="1" t="s">
         <v>247</v>
       </c>
@@ -8437,8 +9109,11 @@
       <c r="M248" s="15">
         <v>1.3667E-2</v>
       </c>
-    </row>
-    <row r="249" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N248" s="16">
+        <v>-2.2811999999999999E-2</v>
+      </c>
+    </row>
+    <row r="249" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A249" s="1" t="s">
         <v>248</v>
       </c>
@@ -8478,8 +9153,11 @@
       <c r="M249" s="15">
         <v>-1.1341E-2</v>
       </c>
-    </row>
-    <row r="250" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N249" s="16">
+        <v>-1.6275000000000001E-2</v>
+      </c>
+    </row>
+    <row r="250" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A250" s="1" t="s">
         <v>249</v>
       </c>
@@ -8519,8 +9197,11 @@
       <c r="M250" s="15">
         <v>-1.3833E-2</v>
       </c>
-    </row>
-    <row r="251" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N250" s="16">
+        <v>-1.0970000000000001E-2</v>
+      </c>
+    </row>
+    <row r="251" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A251" s="1" t="s">
         <v>250</v>
       </c>
@@ -8560,8 +9241,11 @@
       <c r="M251" s="15">
         <v>-2.8722000000000001E-2</v>
       </c>
-    </row>
-    <row r="252" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N251" s="16">
+        <v>-0.118121</v>
+      </c>
+    </row>
+    <row r="252" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A252" s="1" t="s">
         <v>251</v>
       </c>
@@ -8601,8 +9285,11 @@
       <c r="M252" s="15">
         <v>-5.0489999999999997E-3</v>
       </c>
-    </row>
-    <row r="253" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N252" s="16">
+        <v>-0.16009499999999999</v>
+      </c>
+    </row>
+    <row r="253" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A253" s="1" t="s">
         <v>252</v>
       </c>
@@ -8642,8 +9329,11 @@
       <c r="M253" s="15">
         <v>-1.5200000000000001E-4</v>
       </c>
-    </row>
-    <row r="254" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N253" s="16">
+        <v>-2.7518999999999998E-2</v>
+      </c>
+    </row>
+    <row r="254" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A254" s="1" t="s">
         <v>253</v>
       </c>
@@ -8683,8 +9373,11 @@
       <c r="M254" s="15">
         <v>-2.5564E-2</v>
       </c>
-    </row>
-    <row r="255" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N254" s="16">
+        <v>1.0988E-2</v>
+      </c>
+    </row>
+    <row r="255" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A255" s="1" t="s">
         <v>254</v>
       </c>
@@ -8724,8 +9417,11 @@
       <c r="M255" s="15">
         <v>1.5139999999999999E-3</v>
       </c>
-    </row>
-    <row r="256" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N255" s="16">
+        <v>4.8420999999999999E-2</v>
+      </c>
+    </row>
+    <row r="256" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A256" s="1" t="s">
         <v>255</v>
       </c>
@@ -8765,8 +9461,11 @@
       <c r="M256" s="15">
         <v>-8.8679999999999991E-3</v>
       </c>
-    </row>
-    <row r="257" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N256" s="16">
+        <v>2.3552E-2</v>
+      </c>
+    </row>
+    <row r="257" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A257" s="1" t="s">
         <v>256</v>
       </c>
@@ -8806,8 +9505,11 @@
       <c r="M257" s="15">
         <v>6.7599999999999995E-4</v>
       </c>
-    </row>
-    <row r="258" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N257" s="16">
+        <v>3.4604000000000003E-2</v>
+      </c>
+    </row>
+    <row r="258" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A258" s="1" t="s">
         <v>257</v>
       </c>
@@ -8847,8 +9549,11 @@
       <c r="M258" s="15">
         <v>-3.6740000000000002E-3</v>
       </c>
-    </row>
-    <row r="259" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N258" s="16">
+        <v>6.0347999999999999E-2</v>
+      </c>
+    </row>
+    <row r="259" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A259" s="1" t="s">
         <v>258</v>
       </c>
@@ -8888,8 +9593,11 @@
       <c r="M259" s="15">
         <v>1.1172E-2</v>
       </c>
-    </row>
-    <row r="260" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N259" s="16">
+        <v>9.7434999999999994E-2</v>
+      </c>
+    </row>
+    <row r="260" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A260" s="1" t="s">
         <v>259</v>
       </c>
@@ -8929,8 +9637,11 @@
       <c r="M260" s="15">
         <v>1.5790000000000001E-3</v>
       </c>
-    </row>
-    <row r="261" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N260" s="16">
+        <v>2.7928000000000001E-2</v>
+      </c>
+    </row>
+    <row r="261" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A261" s="1" t="s">
         <v>260</v>
       </c>
@@ -8970,8 +9681,11 @@
       <c r="M261" s="15">
         <v>2.676E-3</v>
       </c>
-    </row>
-    <row r="262" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N261" s="16">
+        <v>6.9524000000000002E-2</v>
+      </c>
+    </row>
+    <row r="262" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A262" s="1" t="s">
         <v>261</v>
       </c>
@@ -9011,8 +9725,11 @@
       <c r="M262" s="15">
         <v>5.1359999999999999E-3</v>
       </c>
-    </row>
-    <row r="263" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N262" s="16">
+        <v>3.4202999999999997E-2</v>
+      </c>
+    </row>
+    <row r="263" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A263" s="1" t="s">
         <v>262</v>
       </c>
@@ -9052,8 +9769,11 @@
       <c r="M263" s="15">
         <v>3.0720000000000001E-3</v>
       </c>
-    </row>
-    <row r="264" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N263" s="16">
+        <v>4.3482E-2</v>
+      </c>
+    </row>
+    <row r="264" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A264" s="1" t="s">
         <v>263</v>
       </c>
@@ -9093,8 +9813,11 @@
       <c r="M264" s="15">
         <v>-9.859999999999999E-4</v>
       </c>
-    </row>
-    <row r="265" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N264" s="16">
+        <v>6.8529999999999997E-3</v>
+      </c>
+    </row>
+    <row r="265" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A265" s="1" t="s">
         <v>264</v>
       </c>
@@ -9134,8 +9857,11 @@
       <c r="M265" s="15">
         <v>-3.4329999999999999E-3</v>
       </c>
-    </row>
-    <row r="266" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N265" s="16">
+        <v>9.9279999999999993E-3</v>
+      </c>
+    </row>
+    <row r="266" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A266" s="1" t="s">
         <v>265</v>
       </c>
@@ -9175,8 +9901,11 @@
       <c r="M266" s="15">
         <v>5.4729999999999996E-3</v>
       </c>
-    </row>
-    <row r="267" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N266" s="16">
+        <v>2.7621E-2</v>
+      </c>
+    </row>
+    <row r="267" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A267" s="1" t="s">
         <v>266</v>
       </c>
@@ -9216,8 +9945,11 @@
       <c r="M267" s="15">
         <v>-2.0339999999999998E-3</v>
       </c>
-    </row>
-    <row r="268" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N267" s="16">
+        <v>7.45E-4</v>
+      </c>
+    </row>
+    <row r="268" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A268" s="1" t="s">
         <v>267</v>
       </c>
@@ -9257,8 +9989,11 @@
       <c r="M268" s="15">
         <v>4.365E-3</v>
       </c>
-    </row>
-    <row r="269" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N268" s="16">
+        <v>4.3210000000000002E-3</v>
+      </c>
+    </row>
+    <row r="269" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A269" s="1" t="s">
         <v>268</v>
       </c>
@@ -9298,8 +10033,11 @@
       <c r="M269" s="15">
         <v>5.9249999999999997E-3</v>
       </c>
-    </row>
-    <row r="270" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N269" s="16">
+        <v>2.4523E-2</v>
+      </c>
+    </row>
+    <row r="270" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A270" s="1" t="s">
         <v>269</v>
       </c>
@@ -9339,8 +10077,11 @@
       <c r="M270" s="15">
         <v>-7.4700000000000005E-4</v>
       </c>
-    </row>
-    <row r="271" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N270" s="16">
+        <v>1.9946999999999999E-2</v>
+      </c>
+    </row>
+    <row r="271" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A271" s="1" t="s">
         <v>270</v>
       </c>
@@ -9380,8 +10121,11 @@
       <c r="M271" s="15">
         <v>-6.7669999999999996E-3</v>
       </c>
-    </row>
-    <row r="272" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N271" s="16">
+        <v>-2.6599000000000001E-2</v>
+      </c>
+    </row>
+    <row r="272" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A272" s="1" t="s">
         <v>271</v>
       </c>
@@ -9421,8 +10165,11 @@
       <c r="M272" s="15">
         <v>-6.4739999999999997E-3</v>
       </c>
-    </row>
-    <row r="273" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N272" s="16">
+        <v>1.787E-3</v>
+      </c>
+    </row>
+    <row r="273" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A273" s="1" t="s">
         <v>272</v>
       </c>
@@ -9462,8 +10209,11 @@
       <c r="M273" s="15">
         <v>8.8710000000000004E-3</v>
       </c>
-    </row>
-    <row r="274" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N273" s="16">
+        <v>2.6461999999999999E-2</v>
+      </c>
+    </row>
+    <row r="274" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A274" s="1" t="s">
         <v>273</v>
       </c>
@@ -9503,8 +10253,11 @@
       <c r="M274" s="15">
         <v>-6.9569999999999996E-3</v>
       </c>
-    </row>
-    <row r="275" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N274" s="16">
+        <v>1.2171E-2</v>
+      </c>
+    </row>
+    <row r="275" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A275" s="1" t="s">
         <v>274</v>
       </c>
@@ -9544,8 +10297,11 @@
       <c r="M275" s="15">
         <v>1.1748E-2</v>
       </c>
-    </row>
-    <row r="276" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N275" s="16">
+        <v>2.2369E-2</v>
+      </c>
+    </row>
+    <row r="276" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A276" s="1" t="s">
         <v>275</v>
       </c>
@@ -9585,8 +10341,11 @@
       <c r="M276" s="15">
         <v>8.6540000000000002E-3</v>
       </c>
-    </row>
-    <row r="277" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N276" s="16">
+        <v>2.0160999999999998E-2</v>
+      </c>
+    </row>
+    <row r="277" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A277" s="1" t="s">
         <v>276</v>
       </c>
@@ -9626,8 +10385,11 @@
       <c r="M277" s="15">
         <v>2.5850000000000001E-3</v>
       </c>
-    </row>
-    <row r="278" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N277" s="16">
+        <v>-1.916E-3</v>
+      </c>
+    </row>
+    <row r="278" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A278" s="1" t="s">
         <v>277</v>
       </c>
@@ -9667,8 +10429,11 @@
       <c r="M278" s="15">
         <v>9.2540000000000001E-3</v>
       </c>
-    </row>
-    <row r="279" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N278" s="16">
+        <v>2.3324000000000001E-2</v>
+      </c>
+    </row>
+    <row r="279" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A279" s="1" t="s">
         <v>278</v>
       </c>
@@ -9708,8 +10473,11 @@
       <c r="M279" s="15">
         <v>7.2870000000000001E-3</v>
       </c>
-    </row>
-    <row r="280" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N279" s="16">
+        <v>1.6792999999999999E-2</v>
+      </c>
+    </row>
+    <row r="280" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A280" s="1" t="s">
         <v>279</v>
       </c>
@@ -9749,8 +10517,11 @@
       <c r="M280" s="15">
         <v>4.6800000000000001E-3</v>
       </c>
-    </row>
-    <row r="281" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N280" s="16">
+        <v>7.502E-3</v>
+      </c>
+    </row>
+    <row r="281" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A281" s="1" t="s">
         <v>280</v>
       </c>
@@ -9790,8 +10561,11 @@
       <c r="M281" s="15">
         <v>4.0379999999999999E-3</v>
       </c>
-    </row>
-    <row r="282" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N281" s="16">
+        <v>3.8660000000000001E-3</v>
+      </c>
+    </row>
+    <row r="282" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A282" s="1" t="s">
         <v>281</v>
       </c>
@@ -9831,8 +10605,11 @@
       <c r="M282" s="15">
         <v>3.5309999999999999E-3</v>
       </c>
-    </row>
-    <row r="283" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N282" s="16">
+        <v>-1.9819999999999998E-3</v>
+      </c>
+    </row>
+    <row r="283" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A283" s="1" t="s">
         <v>282</v>
       </c>
@@ -9872,8 +10649,11 @@
       <c r="M283" s="15">
         <v>-4.0330000000000001E-3</v>
       </c>
-    </row>
-    <row r="284" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N283" s="16">
+        <v>-7.7470000000000004E-3</v>
+      </c>
+    </row>
+    <row r="284" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A284" s="1" t="s">
         <v>283</v>
       </c>
@@ -9913,8 +10693,11 @@
       <c r="M284" s="15">
         <v>-1.1670000000000001E-3</v>
       </c>
-    </row>
-    <row r="285" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N284" s="16">
+        <v>-1.4338E-2</v>
+      </c>
+    </row>
+    <row r="285" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A285" s="1" t="s">
         <v>284</v>
       </c>
@@ -9954,8 +10737,11 @@
       <c r="M285" s="15">
         <v>-2.614E-3</v>
       </c>
-    </row>
-    <row r="286" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N285" s="16">
+        <v>-6.2649999999999997E-3</v>
+      </c>
+    </row>
+    <row r="286" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A286" s="1" t="s">
         <v>285</v>
       </c>
@@ -9995,8 +10781,11 @@
       <c r="M286" s="15">
         <v>-2.4549999999999999E-2</v>
       </c>
-    </row>
-    <row r="287" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N286" s="16">
+        <v>-3.3861000000000002E-2</v>
+      </c>
+    </row>
+    <row r="287" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A287" s="1" t="s">
         <v>286</v>
       </c>
@@ -10036,8 +10825,11 @@
       <c r="M287" s="15">
         <v>-2.7636000000000001E-2</v>
       </c>
-    </row>
-    <row r="288" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N287" s="16">
+        <v>-2.9704000000000001E-2</v>
+      </c>
+    </row>
+    <row r="288" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A288" s="1" t="s">
         <v>287</v>
       </c>
@@ -10077,8 +10869,11 @@
       <c r="M288" s="15">
         <v>1.8452E-2</v>
       </c>
-    </row>
-    <row r="289" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N288" s="16">
+        <v>2.3199000000000001E-2</v>
+      </c>
+    </row>
+    <row r="289" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A289" s="1" t="s">
         <v>288</v>
       </c>
@@ -10118,8 +10913,11 @@
       <c r="M289" s="15">
         <v>-1.8109999999999999E-3</v>
       </c>
-    </row>
-    <row r="290" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N289" s="16">
+        <v>-1.3256E-2</v>
+      </c>
+    </row>
+    <row r="290" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A290" s="1" t="s">
         <v>289</v>
       </c>
@@ -10159,8 +10957,11 @@
       <c r="M290" s="15">
         <v>3.235E-3</v>
       </c>
-    </row>
-    <row r="291" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N290" s="16">
+        <v>4.5919999999999997E-3</v>
+      </c>
+    </row>
+    <row r="291" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A291" s="1" t="s">
         <v>290</v>
       </c>
@@ -10200,8 +11001,11 @@
       <c r="M291" s="15">
         <v>1.2337000000000001E-2</v>
       </c>
-    </row>
-    <row r="292" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N291" s="16">
+        <v>2.8104000000000001E-2</v>
+      </c>
+    </row>
+    <row r="292" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A292" s="1" t="s">
         <v>291</v>
       </c>
@@ -10241,8 +11045,11 @@
       <c r="M292" s="15">
         <v>4.8419999999999999E-3</v>
       </c>
-    </row>
-    <row r="293" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N292" s="16">
+        <v>2.529E-2</v>
+      </c>
+    </row>
+    <row r="293" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A293" s="1" t="s">
         <v>292</v>
       </c>
@@ -10282,8 +11089,11 @@
       <c r="M293" s="15">
         <v>-4.08E-4</v>
       </c>
-    </row>
-    <row r="294" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N293" s="16">
+        <v>8.4060000000000003E-3</v>
+      </c>
+    </row>
+    <row r="294" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A294" s="1" t="s">
         <v>293</v>
       </c>
@@ -10323,8 +11133,11 @@
       <c r="M294" s="15">
         <v>-2.738E-3</v>
       </c>
-    </row>
-    <row r="295" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N294" s="16">
+        <v>-9.7429999999999999E-3</v>
+      </c>
+    </row>
+    <row r="295" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A295" s="1" t="s">
         <v>294</v>
       </c>
@@ -10364,8 +11177,11 @@
       <c r="M295" s="15">
         <v>-7.9649999999999999E-3</v>
       </c>
-    </row>
-    <row r="296" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N295" s="16">
+        <v>-1.9779000000000001E-2</v>
+      </c>
+    </row>
+    <row r="296" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A296" s="1" t="s">
         <v>295</v>
       </c>
@@ -10405,8 +11221,11 @@
       <c r="M296" s="15">
         <v>2.8050000000000002E-3</v>
       </c>
-    </row>
-    <row r="297" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N296" s="16">
+        <v>6.9880000000000003E-3</v>
+      </c>
+    </row>
+    <row r="297" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A297" s="1" t="s">
         <v>296</v>
       </c>
@@ -10446,8 +11265,11 @@
       <c r="M297" s="15">
         <v>5.267E-3</v>
       </c>
-    </row>
-    <row r="298" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N297" s="16">
+        <v>9.3080000000000003E-3</v>
+      </c>
+    </row>
+    <row r="298" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A298" s="1" t="s">
         <v>297</v>
       </c>
@@ -10487,8 +11309,11 @@
       <c r="M298" s="15">
         <v>4.0699999999999998E-3</v>
       </c>
-    </row>
-    <row r="299" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N298" s="16">
+        <v>8.907E-3</v>
+      </c>
+    </row>
+    <row r="299" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A299" s="1" t="s">
         <v>298</v>
       </c>
@@ -10528,8 +11353,11 @@
       <c r="M299" s="15">
         <v>2.3080000000000002E-3</v>
       </c>
-    </row>
-    <row r="300" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N299" s="16">
+        <v>8.0839999999999992E-3</v>
+      </c>
+    </row>
+    <row r="300" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A300" s="1" t="s">
         <v>299</v>
       </c>
@@ -10569,8 +11397,11 @@
       <c r="M300" s="15">
         <v>3.2390000000000001E-3</v>
       </c>
-    </row>
-    <row r="301" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N300" s="16">
+        <v>-1.76E-4</v>
+      </c>
+    </row>
+    <row r="301" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A301" s="1" t="s">
         <v>300</v>
       </c>
@@ -10610,8 +11441,11 @@
       <c r="M301" s="15">
         <v>3.7079999999999999E-3</v>
       </c>
-    </row>
-    <row r="302" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N301" s="16">
+        <v>6.4489999999999999E-3</v>
+      </c>
+    </row>
+    <row r="302" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A302" s="1" t="s">
         <v>301</v>
       </c>
@@ -10651,8 +11485,11 @@
       <c r="M302" s="15">
         <v>2.0739999999999999E-3</v>
       </c>
-    </row>
-    <row r="303" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N302" s="16">
+        <v>1.1733E-2</v>
+      </c>
+    </row>
+    <row r="303" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A303" s="1" t="s">
         <v>302</v>
       </c>
@@ -10692,8 +11529,11 @@
       <c r="M303" s="15">
         <v>1.2133E-2</v>
       </c>
-    </row>
-    <row r="304" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N303" s="16">
+        <v>1.7092E-2</v>
+      </c>
+    </row>
+    <row r="304" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A304" s="1" t="s">
         <v>303</v>
       </c>
@@ -10733,8 +11573,11 @@
       <c r="M304" s="15">
         <v>4.2090000000000001E-3</v>
       </c>
-    </row>
-    <row r="305" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N304" s="16">
+        <v>3.663E-3</v>
+      </c>
+    </row>
+    <row r="305" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A305" s="1" t="s">
         <v>304</v>
       </c>
@@ -10774,8 +11617,11 @@
       <c r="M305" s="15">
         <v>3.4259999999999998E-3</v>
       </c>
-    </row>
-    <row r="306" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N305" s="16">
+        <v>8.3510000000000008E-3</v>
+      </c>
+    </row>
+    <row r="306" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A306" s="1" t="s">
         <v>305</v>
       </c>
@@ -10815,8 +11661,11 @@
       <c r="M306" s="15">
         <v>4.4089999999999997E-3</v>
       </c>
-    </row>
-    <row r="307" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N306" s="16">
+        <v>1.0262E-2</v>
+      </c>
+    </row>
+    <row r="307" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A307" s="1" t="s">
         <v>306</v>
       </c>
@@ -10856,8 +11705,11 @@
       <c r="M307" s="15">
         <v>3.2230000000000002E-3</v>
       </c>
-    </row>
-    <row r="308" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N307" s="16">
+        <v>1.4097E-2</v>
+      </c>
+    </row>
+    <row r="308" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A308" s="1" t="s">
         <v>307</v>
       </c>
@@ -10897,8 +11749,11 @@
       <c r="M308" s="15">
         <v>-8.8999999999999995E-5</v>
       </c>
-    </row>
-    <row r="309" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N308" s="16">
+        <v>-1.0544E-2</v>
+      </c>
+    </row>
+    <row r="309" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A309" s="1" t="s">
         <v>308</v>
       </c>
@@ -10938,8 +11793,11 @@
       <c r="M309" s="15">
         <v>1.0789E-2</v>
       </c>
-    </row>
-    <row r="310" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N309" s="16">
+        <v>7.9410000000000001E-3</v>
+      </c>
+    </row>
+    <row r="310" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A310" s="1" t="s">
         <v>309</v>
       </c>
@@ -10979,8 +11837,11 @@
       <c r="M310" s="15">
         <v>-4.5580000000000004E-3</v>
       </c>
-    </row>
-    <row r="311" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N310" s="16">
+        <v>5.5199999999999997E-4</v>
+      </c>
+    </row>
+    <row r="311" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A311" s="1" t="s">
         <v>310</v>
       </c>
@@ -11020,8 +11881,11 @@
       <c r="M311" s="15">
         <v>4.0299999999999997E-3</v>
       </c>
-    </row>
-    <row r="312" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N311" s="16">
+        <v>1.1577E-2</v>
+      </c>
+    </row>
+    <row r="312" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A312" s="1" t="s">
         <v>311</v>
       </c>
@@ -11061,8 +11925,11 @@
       <c r="M312" s="15">
         <v>1.3724E-2</v>
       </c>
-    </row>
-    <row r="313" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N312" s="16">
+        <v>9.162E-3</v>
+      </c>
+    </row>
+    <row r="313" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A313" s="1" t="s">
         <v>312</v>
       </c>
@@ -11102,8 +11969,11 @@
       <c r="M313" s="15">
         <v>8.5360000000000002E-3</v>
       </c>
-    </row>
-    <row r="314" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N313" s="16">
+        <v>3.1300000000000002E-4</v>
+      </c>
+    </row>
+    <row r="314" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A314" s="1" t="s">
         <v>313</v>
       </c>
@@ -11143,8 +12013,11 @@
       <c r="M314" s="15">
         <v>3.091E-3</v>
       </c>
-    </row>
-    <row r="315" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N314" s="16">
+        <v>5.2610000000000001E-3</v>
+      </c>
+    </row>
+    <row r="315" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A315" s="1" t="s">
         <v>314</v>
       </c>
@@ -11184,8 +12057,11 @@
       <c r="M315" s="15">
         <v>6.7000000000000002E-5</v>
       </c>
-    </row>
-    <row r="316" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N315" s="16">
+        <v>8.5609999999999992E-3</v>
+      </c>
+    </row>
+    <row r="316" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A316" s="1" t="s">
         <v>315</v>
       </c>
@@ -11225,8 +12101,11 @@
       <c r="M316" s="15">
         <v>9.1710000000000003E-3</v>
       </c>
-    </row>
-    <row r="317" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N316" s="16">
+        <v>1.1996E-2</v>
+      </c>
+    </row>
+    <row r="317" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A317" s="1" t="s">
         <v>316</v>
       </c>
@@ -11266,8 +12145,11 @@
       <c r="M317" s="15">
         <v>2.8969999999999998E-3</v>
       </c>
-    </row>
-    <row r="318" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N317" s="16">
+        <v>1.851E-3</v>
+      </c>
+    </row>
+    <row r="318" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A318" s="1" t="s">
         <v>317</v>
       </c>
@@ -11307,8 +12189,11 @@
       <c r="M318" s="15">
         <v>3.5820000000000001E-3</v>
       </c>
-    </row>
-    <row r="319" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N318" s="16">
+        <v>1.818E-3</v>
+      </c>
+    </row>
+    <row r="319" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A319" s="1" t="s">
         <v>318</v>
       </c>
@@ -11348,8 +12233,11 @@
       <c r="M319" s="15">
         <v>2.0400000000000001E-3</v>
       </c>
-    </row>
-    <row r="320" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N319" s="16">
+        <v>4.0590000000000001E-3</v>
+      </c>
+    </row>
+    <row r="320" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A320" s="1" t="s">
         <v>319</v>
       </c>
@@ -11389,8 +12277,11 @@
       <c r="M320" s="15">
         <v>-1.1100000000000001E-3</v>
       </c>
-    </row>
-    <row r="321" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N320" s="16">
+        <v>5.5999999999999999E-3</v>
+      </c>
+    </row>
+    <row r="321" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A321" s="1" t="s">
         <v>320</v>
       </c>
@@ -11430,8 +12321,11 @@
       <c r="M321" s="15">
         <v>-1.369E-3</v>
       </c>
-    </row>
-    <row r="322" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N321" s="16">
+        <v>-1.933E-3</v>
+      </c>
+    </row>
+    <row r="322" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A322" s="1" t="s">
         <v>321</v>
       </c>
@@ -11471,8 +12365,11 @@
       <c r="M322" s="15">
         <v>6.1900000000000002E-3</v>
       </c>
-    </row>
-    <row r="323" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N322" s="16">
+        <v>1.547E-3</v>
+      </c>
+    </row>
+    <row r="323" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A323" s="1" t="s">
         <v>322</v>
       </c>
@@ -11512,8 +12409,11 @@
       <c r="M323" s="15">
         <v>-2.8570000000000002E-3</v>
       </c>
-    </row>
-    <row r="324" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N323" s="16">
+        <v>-1.1502999999999999E-2</v>
+      </c>
+    </row>
+    <row r="324" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A324" s="1" t="s">
         <v>323</v>
       </c>
@@ -11553,8 +12453,11 @@
       <c r="M324" s="15">
         <v>5.6300000000000002E-4</v>
       </c>
-    </row>
-    <row r="325" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N324" s="16">
+        <v>-1.2392E-2</v>
+      </c>
+    </row>
+    <row r="325" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A325" s="1" t="s">
         <v>324</v>
       </c>
@@ -11594,8 +12497,11 @@
       <c r="M325" s="15">
         <v>9.3620000000000005E-3</v>
       </c>
-    </row>
-    <row r="326" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N325" s="16">
+        <v>3.5500000000000002E-3</v>
+      </c>
+    </row>
+    <row r="326" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A326" s="1" t="s">
         <v>325</v>
       </c>
@@ -11635,8 +12541,11 @@
       <c r="M326" s="15">
         <v>1.7390000000000001E-3</v>
       </c>
-    </row>
-    <row r="327" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N326" s="16">
+        <v>2.477E-3</v>
+      </c>
+    </row>
+    <row r="327" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A327" s="1" t="s">
         <v>326</v>
       </c>
@@ -11676,8 +12585,11 @@
       <c r="M327" s="15">
         <v>2.307E-3</v>
       </c>
-    </row>
-    <row r="328" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N327" s="16">
+        <v>4.156E-3</v>
+      </c>
+    </row>
+    <row r="328" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A328" s="1" t="s">
         <v>327</v>
       </c>
@@ -11717,8 +12629,11 @@
       <c r="M328" s="15">
         <v>7.9240000000000005E-3</v>
       </c>
-    </row>
-    <row r="329" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N328" s="16">
+        <v>1.3934E-2</v>
+      </c>
+    </row>
+    <row r="329" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A329" s="1" t="s">
         <v>328</v>
       </c>
@@ -11758,8 +12673,11 @@
       <c r="M329" s="15">
         <v>5.4169999999999999E-3</v>
       </c>
-    </row>
-    <row r="330" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N329" s="16">
+        <v>1.8829999999999999E-3</v>
+      </c>
+    </row>
+    <row r="330" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A330" s="1" t="s">
         <v>329</v>
       </c>
@@ -11799,8 +12717,11 @@
       <c r="M330" s="15">
         <v>1.4469999999999999E-3</v>
       </c>
-    </row>
-    <row r="331" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N330" s="16">
+        <v>1.5765999999999999E-2</v>
+      </c>
+    </row>
+    <row r="331" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A331" s="1" t="s">
         <v>330</v>
       </c>
@@ -11840,8 +12761,11 @@
       <c r="M331" s="15">
         <v>4.1460000000000004E-3</v>
       </c>
-    </row>
-    <row r="332" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N331" s="16">
+        <v>6.9519999999999998E-3</v>
+      </c>
+    </row>
+    <row r="332" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A332" s="1" t="s">
         <v>331</v>
       </c>
@@ -11881,8 +12805,11 @@
       <c r="M332" s="15">
         <v>-3.8099999999999999E-4</v>
       </c>
-    </row>
-    <row r="333" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N332" s="16">
+        <v>-8.7460000000000003E-3</v>
+      </c>
+    </row>
+    <row r="333" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A333" s="1" t="s">
         <v>332</v>
       </c>
@@ -11922,8 +12849,11 @@
       <c r="M333" s="15">
         <v>2.6340000000000001E-3</v>
       </c>
-    </row>
-    <row r="334" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N333" s="16">
+        <v>-5.6839999999999998E-3</v>
+      </c>
+    </row>
+    <row r="334" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A334" s="1" t="s">
         <v>333</v>
       </c>
@@ -11963,8 +12893,11 @@
       <c r="M334" s="15">
         <v>-3.79E-3</v>
       </c>
-    </row>
-    <row r="335" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N334" s="16">
+        <v>-6.7010000000000004E-3</v>
+      </c>
+    </row>
+    <row r="335" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A335" s="1" t="s">
         <v>334</v>
       </c>
@@ -12004,8 +12937,11 @@
       <c r="M335" s="15">
         <v>1.1110999999999999E-2</v>
       </c>
-    </row>
-    <row r="336" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N335" s="16">
+        <v>-4.8079999999999998E-3</v>
+      </c>
+    </row>
+    <row r="336" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A336" s="1" t="s">
         <v>335</v>
       </c>
@@ -12045,8 +12981,11 @@
       <c r="M336" s="15">
         <v>1.0352E-2</v>
       </c>
-    </row>
-    <row r="337" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N336" s="16">
+        <v>1.5540999999999999E-2</v>
+      </c>
+    </row>
+    <row r="337" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A337" s="1" t="s">
         <v>336</v>
       </c>
@@ -12086,8 +13025,11 @@
       <c r="M337" s="15">
         <v>1.073E-3</v>
       </c>
-    </row>
-    <row r="338" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N337" s="16">
+        <v>-2.9759999999999999E-3</v>
+      </c>
+    </row>
+    <row r="338" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A338" s="1" t="s">
         <v>337</v>
       </c>
@@ -12127,8 +13069,11 @@
       <c r="M338" s="15">
         <v>-2.4499999999999999E-4</v>
       </c>
-    </row>
-    <row r="339" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N338" s="16">
+        <v>-9.7949999999999999E-3</v>
+      </c>
+    </row>
+    <row r="339" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A339" s="1" t="s">
         <v>338</v>
       </c>
@@ -12168,8 +13113,11 @@
       <c r="M339" s="15">
         <v>3.5500000000000001E-4</v>
       </c>
-    </row>
-    <row r="340" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N339" s="16">
+        <v>-2.1042000000000002E-2</v>
+      </c>
+    </row>
+    <row r="340" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A340" s="1" t="s">
         <v>339</v>
       </c>
@@ -12209,8 +13157,11 @@
       <c r="M340" s="15">
         <v>-6.4689999999999999E-3</v>
       </c>
-    </row>
-    <row r="341" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N340" s="16">
+        <v>6.1499999999999999E-4</v>
+      </c>
+    </row>
+    <row r="341" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A341" s="1" t="s">
         <v>340</v>
       </c>
@@ -12250,8 +13201,11 @@
       <c r="M341" s="15">
         <v>1.1305000000000001E-2</v>
       </c>
-    </row>
-    <row r="342" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N341" s="16">
+        <v>1.6452999999999999E-2</v>
+      </c>
+    </row>
+    <row r="342" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A342" s="1" t="s">
         <v>341</v>
       </c>
@@ -12291,8 +13245,11 @@
       <c r="M342" s="15">
         <v>-8.8129999999999997E-3</v>
       </c>
-    </row>
-    <row r="343" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N342" s="16">
+        <v>1.4872E-2</v>
+      </c>
+    </row>
+    <row r="343" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A343" s="1" t="s">
         <v>342</v>
       </c>
@@ -12332,8 +13289,11 @@
       <c r="M343" s="15">
         <v>4.8129999999999996E-3</v>
       </c>
-    </row>
-    <row r="344" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N343" s="16">
+        <v>1.3035E-2</v>
+      </c>
+    </row>
+    <row r="344" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A344" s="1" t="s">
         <v>343</v>
       </c>
@@ -12373,8 +13333,11 @@
       <c r="M344" s="15">
         <v>3.8000000000000002E-4</v>
       </c>
-    </row>
-    <row r="345" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N344" s="16">
+        <v>-1.65E-4</v>
+      </c>
+    </row>
+    <row r="345" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A345" s="1" t="s">
         <v>344</v>
       </c>
@@ -12414,8 +13377,11 @@
       <c r="M345" s="15">
         <v>8.4759999999999992E-3</v>
       </c>
-    </row>
-    <row r="346" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N345" s="16">
+        <v>1.5928000000000001E-2</v>
+      </c>
+    </row>
+    <row r="346" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A346" s="1" t="s">
         <v>345</v>
       </c>
@@ -12455,8 +13421,11 @@
       <c r="M346" s="15">
         <v>-2.4689999999999998E-3</v>
       </c>
-    </row>
-    <row r="347" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N346" s="16">
+        <v>1.2547000000000001E-2</v>
+      </c>
+    </row>
+    <row r="347" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A347" s="1" t="s">
         <v>346</v>
       </c>
@@ -12496,8 +13465,11 @@
       <c r="M347" s="15">
         <v>8.3199999999999995E-4</v>
       </c>
-    </row>
-    <row r="348" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N347" s="16">
+        <v>6.1199999999999996E-3</v>
+      </c>
+    </row>
+    <row r="348" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A348" s="1" t="s">
         <v>347</v>
       </c>
@@ -12537,8 +13509,11 @@
       <c r="M348" s="15">
         <v>-9.0700000000000004E-4</v>
       </c>
-    </row>
-    <row r="349" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N348" s="16">
+        <v>3.3779999999999999E-3</v>
+      </c>
+    </row>
+    <row r="349" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A349" s="1" t="s">
         <v>348</v>
       </c>
@@ -12578,8 +13553,11 @@
       <c r="M349" s="15" t="s">
         <v>350</v>
       </c>
-    </row>
-    <row r="350" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N349" s="16" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="350" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A350" s="1" t="s">
         <v>349</v>
       </c>
@@ -12617,6 +13595,9 @@
         <v>350</v>
       </c>
       <c r="M350" s="15" t="s">
+        <v>350</v>
+      </c>
+      <c r="N350" s="16" t="s">
         <v>350</v>
       </c>
     </row>

</xml_diff>